<commit_message>
add peak uncertainty to Fe files
</commit_message>
<xml_diff>
--- a/csdata/Fe/SI/Fe14+.xlsx
+++ b/csdata/Fe/SI/Fe14+.xlsx
@@ -1,17 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmondeel/Documents/CfA/Chandra/CHANDRA-Rates/csdata/Fe/SI/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C954F63-3698-C14E-8A1C-3B3064E55599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Energy (eV)</t>
   </si>
@@ -30,35 +52,51 @@
   <si>
     <t>Absolute rate coefficients for photorecombination and electron-impact ionization of magnesiumlike iron ions from measurements at a heavy-ion storage ring Bernhardt 2014</t>
   </si>
+  <si>
+    <t>Unc at peak</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -67,57 +105,56 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -307,20 +344,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z524"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -336,22 +378,29 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="F1" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
-        <v>419.5083495</v>
+        <v>419.50834950000001</v>
       </c>
       <c r="B2" s="4">
-        <v>-0.009940357853</v>
+        <v>-9.9403578530000009E-3</v>
       </c>
       <c r="C2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>-19.0</v>
+        <v>0</v>
+      </c>
+      <c r="D2" s="10">
+        <v>-19</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>5</v>
+      </c>
+      <c r="F2">
+        <f>_xlfn.XLOOKUP(MAX(B:B),B:B,C:C)/MAX(B:B)</f>
+        <v>0.2598364184497301</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -372,15 +421,15 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
-        <v>449.5100914</v>
+        <v>449.51009140000002</v>
       </c>
       <c r="B3" s="4">
-        <v>-0.009940357853</v>
+        <v>-9.9403578530000009E-3</v>
       </c>
       <c r="C3" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D3" s="5"/>
       <c r="G3" s="2"/>
@@ -404,12 +453,12 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
-        <v>462.6355068</v>
+        <v>462.63550679999997</v>
       </c>
       <c r="B4" s="4">
-        <v>0.04572564612</v>
+        <v>4.5725646119999998E-2</v>
       </c>
       <c r="C4" s="5">
         <v>0.01</v>
@@ -436,12 +485,12 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
-        <v>472.5037642</v>
+        <v>472.50376419999998</v>
       </c>
       <c r="B5" s="4">
-        <v>0.1013916501</v>
+        <v>0.10139165009999999</v>
       </c>
       <c r="C5" s="5">
         <v>0.03</v>
@@ -468,12 +517,12 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
-        <v>483.5093591</v>
+        <v>483.50935909999998</v>
       </c>
       <c r="B6" s="4">
-        <v>0.2127236581</v>
+        <v>0.21272365809999999</v>
       </c>
       <c r="C6" s="5">
         <v>0.06</v>
@@ -500,12 +549,12 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
-        <v>493.8228667</v>
+        <v>493.82286670000002</v>
       </c>
       <c r="B7" s="4">
-        <v>0.2445328032</v>
+        <v>0.24453280320000001</v>
       </c>
       <c r="C7" s="5">
         <v>0.06</v>
@@ -532,12 +581,12 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
-        <v>507.2679346</v>
+        <v>507.26793459999999</v>
       </c>
       <c r="B8" s="4">
-        <v>0.3399602386</v>
+        <v>0.33996023860000002</v>
       </c>
       <c r="C8" s="5">
         <v>0.09</v>
@@ -564,7 +613,7 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>521.0790647</v>
       </c>
@@ -596,12 +645,12 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
-        <v>533.2160794</v>
+        <v>533.21607940000001</v>
       </c>
       <c r="B10" s="4">
-        <v>0.4831013917</v>
+        <v>0.48310139169999999</v>
       </c>
       <c r="C10" s="5">
         <v>0.13</v>
@@ -628,15 +677,15 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
-        <v>545.6357903</v>
+        <v>545.63579030000005</v>
       </c>
       <c r="B11" s="4">
-        <v>0.5467196819</v>
+        <v>0.54671968189999998</v>
       </c>
       <c r="C11" s="5">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D11" s="5"/>
       <c r="G11" s="2"/>
@@ -660,12 +709,12 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
-        <v>555.1400483</v>
+        <v>555.14004829999999</v>
       </c>
       <c r="B12" s="4">
-        <v>0.6103379722</v>
+        <v>0.61033797219999997</v>
       </c>
       <c r="C12" s="5">
         <v>0.16</v>
@@ -692,12 +741,12 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
-        <v>566.9814759</v>
+        <v>566.98147589999996</v>
       </c>
       <c r="B13" s="4">
-        <v>0.6421471173</v>
+        <v>0.64214711729999996</v>
       </c>
       <c r="C13" s="5">
         <v>0.17</v>
@@ -724,12 +773,12 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
-        <v>580.1876531</v>
+        <v>580.18765310000003</v>
       </c>
       <c r="B14" s="4">
-        <v>0.7057654076</v>
+        <v>0.70576540759999995</v>
       </c>
       <c r="C14" s="5">
         <v>0.18</v>
@@ -756,12 +805,12 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
-        <v>593.7014297</v>
+        <v>593.70142969999995</v>
       </c>
       <c r="B15" s="4">
-        <v>0.7534791252</v>
+        <v>0.75347912520000004</v>
       </c>
       <c r="C15" s="5">
         <v>0.2</v>
@@ -788,12 +837,12 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
-        <v>605.2030458</v>
+        <v>605.20304580000004</v>
       </c>
       <c r="B16" s="4">
-        <v>0.8330019881</v>
+        <v>0.83300198810000003</v>
       </c>
       <c r="C16" s="5">
         <v>0.22</v>
@@ -820,12 +869,12 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
-        <v>615.744887</v>
+        <v>615.74488699999995</v>
       </c>
       <c r="B17" s="4">
-        <v>0.8011928429</v>
+        <v>0.80119284290000004</v>
       </c>
       <c r="C17" s="5">
         <v>0.21</v>
@@ -852,12 +901,12 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
-        <v>627.673545</v>
+        <v>627.67354499999999</v>
       </c>
       <c r="B18" s="4">
-        <v>0.8330019881</v>
+        <v>0.83300198810000003</v>
       </c>
       <c r="C18" s="5">
         <v>0.22</v>
@@ -884,12 +933,12 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
-        <v>638.6067927</v>
+        <v>638.60679270000003</v>
       </c>
       <c r="B19" s="4">
-        <v>0.8648111332</v>
+        <v>0.86481113320000003</v>
       </c>
       <c r="C19" s="5">
         <v>0.22</v>
@@ -916,12 +965,12 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>647.2419251</v>
       </c>
       <c r="B20" s="4">
-        <v>0.8807157058</v>
+        <v>0.88071570580000003</v>
       </c>
       <c r="C20" s="5">
         <v>0.23</v>
@@ -948,12 +997,12 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
-        <v>653.4812725</v>
+        <v>653.48127250000005</v>
       </c>
       <c r="B21" s="4">
-        <v>0.8807157058</v>
+        <v>0.88071570580000003</v>
       </c>
       <c r="C21" s="5">
         <v>0.23</v>
@@ -980,12 +1029,12 @@
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
-        <v>663.5895744</v>
+        <v>663.58957439999995</v>
       </c>
       <c r="B22" s="4">
-        <v>0.944333996</v>
+        <v>0.94433399600000001</v>
       </c>
       <c r="C22" s="5">
         <v>0.25</v>
@@ -1012,12 +1061,12 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
-        <v>673.8542355</v>
+        <v>673.85423549999996</v>
       </c>
       <c r="B23" s="4">
-        <v>0.944333996</v>
+        <v>0.94433399600000001</v>
       </c>
       <c r="C23" s="5">
         <v>0.25</v>
@@ -1044,12 +1093,12 @@
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
-        <v>682.9659777</v>
+        <v>682.96597770000005</v>
       </c>
       <c r="B24" s="4">
-        <v>0.9125248509</v>
+        <v>0.91252485090000002</v>
       </c>
       <c r="C24" s="5">
         <v>0.24</v>
@@ -1076,12 +1125,12 @@
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>694.862347</v>
       </c>
       <c r="B25" s="4">
-        <v>0.944333996</v>
+        <v>0.94433399600000001</v>
       </c>
       <c r="C25" s="5">
         <v>0.25</v>
@@ -1108,9 +1157,9 @@
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
-        <v>709.6841244</v>
+        <v>709.68412439999997</v>
       </c>
       <c r="B26" s="4">
         <v>0.9920477137</v>
@@ -1140,9 +1189,9 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
-        <v>727.6089014</v>
+        <v>727.60890140000004</v>
       </c>
       <c r="B27" s="4">
         <v>1.294234592</v>
@@ -1172,12 +1221,12 @@
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
-        <v>733.2147746</v>
+        <v>733.21477460000006</v>
       </c>
       <c r="B28" s="4">
-        <v>1.588469185</v>
+        <v>1.5884691849999999</v>
       </c>
       <c r="C28" s="5">
         <v>0.41</v>
@@ -1204,12 +1253,12 @@
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>738.8638383</v>
       </c>
       <c r="B29" s="4">
-        <v>1.89860835</v>
+        <v>1.8986083499999999</v>
       </c>
       <c r="C29" s="5">
         <v>0.49</v>
@@ -1236,12 +1285,12 @@
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
-        <v>753.1776462</v>
+        <v>753.17764620000003</v>
       </c>
       <c r="B30" s="4">
-        <v>1.994035785</v>
+        <v>1.9940357849999999</v>
       </c>
       <c r="C30" s="5">
         <v>0.52</v>
@@ -1268,15 +1317,15 @@
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
-        <v>758.9805141</v>
+        <v>758.98051410000005</v>
       </c>
       <c r="B31" s="4">
-        <v>2.184890656</v>
+        <v>2.1848906559999999</v>
       </c>
       <c r="C31" s="5">
-        <v>0.57</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="D31" s="5"/>
       <c r="G31" s="2"/>
@@ -1300,9 +1349,9 @@
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
-        <v>761.8986922</v>
+        <v>761.89869220000003</v>
       </c>
       <c r="B32" s="4">
         <v>2.614314115</v>
@@ -1332,12 +1381,12 @@
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
-        <v>763.3619861</v>
+        <v>763.36198609999997</v>
       </c>
       <c r="B33" s="4">
-        <v>2.852882704</v>
+        <v>2.8528827040000002</v>
       </c>
       <c r="C33" s="5">
         <v>0.74</v>
@@ -1364,9 +1413,9 @@
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
-        <v>764.8280903</v>
+        <v>764.82809029999999</v>
       </c>
       <c r="B34" s="4">
         <v>3.155069583</v>
@@ -1396,12 +1445,12 @@
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
-        <v>766.2970104</v>
+        <v>766.29701039999998</v>
       </c>
       <c r="B35" s="4">
-        <v>3.473161034</v>
+        <v>3.4731610339999999</v>
       </c>
       <c r="C35" s="5">
         <v>0.9</v>
@@ -1428,12 +1477,12 @@
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
-        <v>767.7687516</v>
+        <v>767.76875159999997</v>
       </c>
       <c r="B36" s="4">
-        <v>3.011928429</v>
+        <v>3.0119284290000001</v>
       </c>
       <c r="C36" s="5">
         <v>0.78</v>
@@ -1460,9 +1509,9 @@
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
-        <v>768.5056818</v>
+        <v>768.50568180000005</v>
       </c>
       <c r="B37" s="4">
         <v>2.741550696</v>
@@ -1492,12 +1541,12 @@
       <c r="Y37" s="2"/>
       <c r="Z37" s="2"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
-        <v>770.7207193</v>
+        <v>770.72071930000004</v>
       </c>
       <c r="B38" s="4">
-        <v>2.566600398</v>
+        <v>2.5666003979999998</v>
       </c>
       <c r="C38" s="5">
         <v>0.67</v>
@@ -1524,9 +1573,9 @@
       <c r="Y38" s="2"/>
       <c r="Z38" s="2"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
-        <v>772.2009566</v>
+        <v>772.20095660000004</v>
       </c>
       <c r="B39" s="4">
         <v>2.964214712</v>
@@ -1556,12 +1605,12 @@
       <c r="Y39" s="2"/>
       <c r="Z39" s="2"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
-        <v>773.6840369</v>
+        <v>773.68403690000002</v>
       </c>
       <c r="B40" s="4">
-        <v>3.425447316</v>
+        <v>3.4254473160000001</v>
       </c>
       <c r="C40" s="5">
         <v>0.89</v>
@@ -1588,12 +1637,12 @@
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
-        <v>776.6587481</v>
+        <v>776.65874810000003</v>
       </c>
       <c r="B41" s="4">
-        <v>3.584493042</v>
+        <v>3.5844930420000001</v>
       </c>
       <c r="C41" s="5">
         <v>0.93</v>
@@ -1620,12 +1669,12 @@
       <c r="Y41" s="2"/>
       <c r="Z41" s="2"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3">
-        <v>778.1503899</v>
+        <v>778.15038990000005</v>
       </c>
       <c r="B42" s="4">
-        <v>3.26640159</v>
+        <v>3.2664015900000001</v>
       </c>
       <c r="C42" s="5">
         <v>0.85</v>
@@ -1652,9 +1701,9 @@
       <c r="Y42" s="2"/>
       <c r="Z42" s="2"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="3">
-        <v>781.1422736</v>
+        <v>781.14227359999995</v>
       </c>
       <c r="B43" s="4">
         <v>2.836978131</v>
@@ -1684,12 +1733,12 @@
       <c r="Y43" s="2"/>
       <c r="Z43" s="2"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="3">
-        <v>785.6516819</v>
+        <v>785.65168189999997</v>
       </c>
       <c r="B44" s="4">
-        <v>3.123260437</v>
+        <v>3.1232604369999999</v>
       </c>
       <c r="C44" s="5">
         <v>0.81</v>
@@ -1716,12 +1765,12 @@
       <c r="Y44" s="2"/>
       <c r="Z44" s="2"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="3">
-        <v>788.672407</v>
+        <v>788.67240700000002</v>
       </c>
       <c r="B45" s="4">
-        <v>3.69582505</v>
+        <v>3.6958250499999998</v>
       </c>
       <c r="C45" s="5">
         <v>0.96</v>
@@ -1748,12 +1797,12 @@
       <c r="Y45" s="2"/>
       <c r="Z45" s="2"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="3">
-        <v>793.2252855</v>
+        <v>793.22528550000004</v>
       </c>
       <c r="B46" s="4">
-        <v>3.091451292</v>
+        <v>3.0914512919999999</v>
       </c>
       <c r="C46" s="5">
         <v>0.8</v>
@@ -1780,12 +1829,12 @@
       <c r="Y46" s="2"/>
       <c r="Z46" s="2"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3">
-        <v>796.2751301</v>
+        <v>796.27513009999996</v>
       </c>
       <c r="B47" s="4">
-        <v>3.345924453</v>
+        <v>3.3459244529999999</v>
       </c>
       <c r="C47" s="5">
         <v>0.87</v>
@@ -1812,12 +1861,12 @@
       <c r="Y47" s="2"/>
       <c r="Z47" s="2"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3">
-        <v>802.4100433</v>
+        <v>802.41004329999998</v>
       </c>
       <c r="B48" s="4">
-        <v>3.330019881</v>
+        <v>3.3300198810000001</v>
       </c>
       <c r="C48" s="5">
         <v>0.87</v>
@@ -1844,12 +1893,12 @@
       <c r="Y48" s="2"/>
       <c r="Z48" s="2"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="3">
-        <v>807.0422269</v>
+        <v>807.04222689999995</v>
       </c>
       <c r="B49" s="4">
-        <v>3.282306163</v>
+        <v>3.2823061629999999</v>
       </c>
       <c r="C49" s="5">
         <v>0.85</v>
@@ -1876,12 +1925,12 @@
       <c r="Y49" s="2"/>
       <c r="Z49" s="2"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="3">
-        <v>811.7011513</v>
+        <v>811.70115129999999</v>
       </c>
       <c r="B50" s="4">
-        <v>3.552683897</v>
+        <v>3.5526838970000001</v>
       </c>
       <c r="C50" s="5">
         <v>0.92</v>
@@ -1908,12 +1957,12 @@
       <c r="Y50" s="2"/>
       <c r="Z50" s="2"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="3">
-        <v>814.8220332</v>
+        <v>814.82203319999996</v>
       </c>
       <c r="B51" s="4">
-        <v>3.425447316</v>
+        <v>3.4254473160000001</v>
       </c>
       <c r="C51" s="5">
         <v>0.89</v>
@@ -1940,12 +1989,12 @@
       <c r="Y51" s="2"/>
       <c r="Z51" s="2"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="3">
-        <v>819.5258693</v>
+        <v>819.52586929999995</v>
       </c>
       <c r="B52" s="4">
-        <v>3.727634195</v>
+        <v>3.7276341949999998</v>
       </c>
       <c r="C52" s="5">
         <v>0.97</v>
@@ -1972,12 +2021,12 @@
       <c r="Y52" s="2"/>
       <c r="Z52" s="2"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="3">
-        <v>824.2568598</v>
+        <v>824.25685980000003</v>
       </c>
       <c r="B53" s="4">
-        <v>3.393638171</v>
+        <v>3.3936381710000001</v>
       </c>
       <c r="C53" s="5">
         <v>0.88</v>
@@ -2004,12 +2053,12 @@
       <c r="Y53" s="2"/>
       <c r="Z53" s="2"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="3">
-        <v>832.2026135</v>
+        <v>832.20261349999998</v>
       </c>
       <c r="B54" s="4">
-        <v>3.552683897</v>
+        <v>3.5526838970000001</v>
       </c>
       <c r="C54" s="5">
         <v>0.92</v>
@@ -2036,12 +2085,12 @@
       <c r="Y54" s="2"/>
       <c r="Z54" s="2"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="3">
-        <v>837.0067848</v>
+        <v>837.00678479999999</v>
       </c>
       <c r="B55" s="4">
-        <v>3.775347913</v>
+        <v>3.7753479130000001</v>
       </c>
       <c r="C55" s="5">
         <v>0.98</v>
@@ -2068,12 +2117,12 @@
       <c r="Y55" s="2"/>
       <c r="Z55" s="2"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="3">
         <v>841.8386898</v>
       </c>
       <c r="B56" s="4">
-        <v>3.473161034</v>
+        <v>3.4731610339999999</v>
       </c>
       <c r="C56" s="5">
         <v>0.9</v>
@@ -2100,7 +2149,7 @@
       <c r="Y56" s="2"/>
       <c r="Z56" s="2"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="3">
         <v>845.0754465</v>
       </c>
@@ -2132,15 +2181,15 @@
       <c r="Y57" s="2"/>
       <c r="Z57" s="2"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="3">
-        <v>848.324648</v>
+        <v>848.32464800000002</v>
       </c>
       <c r="B58" s="4">
-        <v>4.220675944</v>
+        <v>4.2206759439999999</v>
       </c>
       <c r="C58" s="5">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D58" s="5"/>
       <c r="G58" s="2"/>
@@ -2164,12 +2213,12 @@
       <c r="Y58" s="2"/>
       <c r="Z58" s="2"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="3">
-        <v>853.2218893</v>
+        <v>853.22188930000004</v>
       </c>
       <c r="B59" s="4">
-        <v>3.727634195</v>
+        <v>3.7276341949999998</v>
       </c>
       <c r="C59" s="5">
         <v>0.97</v>
@@ -2196,15 +2245,15 @@
       <c r="Y59" s="2"/>
       <c r="Z59" s="2"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="3">
         <v>858.1474015</v>
       </c>
       <c r="B60" s="4">
-        <v>4.37972167</v>
+        <v>4.3797216700000003</v>
       </c>
       <c r="C60" s="5">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="D60" s="5"/>
       <c r="G60" s="2"/>
@@ -2228,9 +2277,9 @@
       <c r="Y60" s="2"/>
       <c r="Z60" s="2"/>
     </row>
-    <row r="61">
+    <row r="61" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="3">
-        <v>861.4468629</v>
+        <v>861.44686290000004</v>
       </c>
       <c r="B61" s="4">
         <v>4.029821074</v>
@@ -2260,12 +2309,12 @@
       <c r="Y61" s="2"/>
       <c r="Z61" s="2"/>
     </row>
-    <row r="62">
+    <row r="62" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="3">
-        <v>868.0838926</v>
+        <v>868.08389260000001</v>
       </c>
       <c r="B62" s="4">
-        <v>3.632206759</v>
+        <v>3.6322067589999998</v>
       </c>
       <c r="C62" s="5">
         <v>0.94</v>
@@ -2292,12 +2341,12 @@
       <c r="Y62" s="2"/>
       <c r="Z62" s="2"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="3">
-        <v>871.4215585</v>
+        <v>871.42155849999995</v>
       </c>
       <c r="B63" s="4">
-        <v>3.82306163</v>
+        <v>3.8230616300000002</v>
       </c>
       <c r="C63" s="5">
         <v>0.99</v>
@@ -2324,12 +2373,12 @@
       <c r="Y63" s="2"/>
       <c r="Z63" s="2"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="3">
-        <v>874.7720573</v>
+        <v>874.77205730000003</v>
       </c>
       <c r="B64" s="4">
-        <v>3.568588469</v>
+        <v>3.5685884689999998</v>
       </c>
       <c r="C64" s="5">
         <v>0.93</v>
@@ -2356,15 +2405,15 @@
       <c r="Y64" s="2"/>
       <c r="Z64" s="2"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="3">
-        <v>881.5117511</v>
+        <v>881.51175109999997</v>
       </c>
       <c r="B65" s="4">
-        <v>4.37972167</v>
+        <v>4.3797216700000003</v>
       </c>
       <c r="C65" s="5">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="D65" s="5"/>
       <c r="G65" s="2"/>
@@ -2388,12 +2437,12 @@
       <c r="Y65" s="2"/>
       <c r="Z65" s="2"/>
     </row>
-    <row r="66">
+    <row r="66" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="3">
-        <v>884.9010454</v>
+        <v>884.90104540000004</v>
       </c>
       <c r="B66" s="4">
-        <v>4.077534791</v>
+        <v>4.0775347909999997</v>
       </c>
       <c r="C66" s="5">
         <v>1.06</v>
@@ -2420,9 +2469,9 @@
       <c r="Y66" s="2"/>
       <c r="Z66" s="2"/>
     </row>
-    <row r="67">
+    <row r="67" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="3">
-        <v>888.303371</v>
+        <v>888.30337099999997</v>
       </c>
       <c r="B67" s="4">
         <v>3.743538767</v>
@@ -2452,12 +2501,12 @@
       <c r="Y67" s="2"/>
       <c r="Z67" s="2"/>
     </row>
-    <row r="68">
+    <row r="68" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="3">
-        <v>891.7187781</v>
+        <v>891.71877810000001</v>
       </c>
       <c r="B68" s="4">
-        <v>3.457256461</v>
+        <v>3.4572564610000001</v>
       </c>
       <c r="C68" s="5">
         <v>0.9</v>
@@ -2484,15 +2533,15 @@
       <c r="Y68" s="2"/>
       <c r="Z68" s="2"/>
     </row>
-    <row r="69">
+    <row r="69" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="3">
-        <v>895.147317</v>
+        <v>895.14731700000004</v>
       </c>
       <c r="B69" s="4">
-        <v>4.236580517</v>
+        <v>4.2365805170000002</v>
       </c>
       <c r="C69" s="5">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D69" s="5"/>
       <c r="G69" s="2"/>
@@ -2516,12 +2565,12 @@
       <c r="Y69" s="2"/>
       <c r="Z69" s="2"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="3">
         <v>898.5890382</v>
       </c>
       <c r="B70" s="4">
-        <v>3.88667992</v>
+        <v>3.8866799200000002</v>
       </c>
       <c r="C70" s="5">
         <v>1.01</v>
@@ -2548,15 +2597,15 @@
       <c r="Y70" s="2"/>
       <c r="Z70" s="2"/>
     </row>
-    <row r="71">
+    <row r="71" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="3">
-        <v>902.0439923</v>
+        <v>902.04399230000001</v>
       </c>
       <c r="B71" s="4">
         <v>4.284294235</v>
       </c>
       <c r="C71" s="5">
-        <v>1.11</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="D71" s="5"/>
       <c r="G71" s="2"/>
@@ -2580,12 +2629,12 @@
       <c r="Y71" s="2"/>
       <c r="Z71" s="2"/>
     </row>
-    <row r="72">
+    <row r="72" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="3">
-        <v>905.5122303</v>
+        <v>905.51223030000006</v>
       </c>
       <c r="B72" s="4">
-        <v>3.982107356</v>
+        <v>3.9821073560000002</v>
       </c>
       <c r="C72" s="5">
         <v>1.04</v>
@@ -2612,12 +2661,12 @@
       <c r="Y72" s="2"/>
       <c r="Z72" s="2"/>
     </row>
-    <row r="73">
+    <row r="73" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="3">
-        <v>908.9938031</v>
+        <v>908.99380310000004</v>
       </c>
       <c r="B73" s="4">
-        <v>3.664015905</v>
+        <v>3.6640159049999999</v>
       </c>
       <c r="C73" s="5">
         <v>0.95</v>
@@ -2644,12 +2693,12 @@
       <c r="Y73" s="2"/>
       <c r="Z73" s="2"/>
     </row>
-    <row r="74">
+    <row r="74" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="3">
-        <v>914.2412776</v>
+        <v>914.24127759999999</v>
       </c>
       <c r="B74" s="4">
-        <v>4.125248509</v>
+        <v>4.1252485090000004</v>
       </c>
       <c r="C74" s="5">
         <v>1.07</v>
@@ -2676,15 +2725,15 @@
       <c r="Y74" s="2"/>
       <c r="Z74" s="2"/>
     </row>
-    <row r="75">
+    <row r="75" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="3">
-        <v>917.7564125</v>
+        <v>917.75641250000001</v>
       </c>
       <c r="B75" s="4">
-        <v>4.236580517</v>
+        <v>4.2365805170000002</v>
       </c>
       <c r="C75" s="5">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D75" s="5"/>
       <c r="G75" s="2"/>
@@ -2708,7 +2757,7 @@
       <c r="Y75" s="2"/>
       <c r="Z75" s="2"/>
     </row>
-    <row r="76">
+    <row r="76" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="3">
         <v>923.0544721</v>
       </c>
@@ -2740,12 +2789,12 @@
       <c r="Y76" s="2"/>
       <c r="Z76" s="2"/>
     </row>
-    <row r="77">
+    <row r="77" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="3">
-        <v>930.1661584</v>
+        <v>930.16615839999997</v>
       </c>
       <c r="B77" s="4">
-        <v>4.157057654</v>
+        <v>4.1570576539999999</v>
       </c>
       <c r="C77" s="5">
         <v>1.08</v>
@@ -2772,9 +2821,9 @@
       <c r="Y77" s="2"/>
       <c r="Z77" s="2"/>
     </row>
-    <row r="78">
+    <row r="78" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="3">
-        <v>935.5358575</v>
+        <v>935.53585750000002</v>
       </c>
       <c r="B78" s="4">
         <v>3.743538767</v>
@@ -2804,12 +2853,12 @@
       <c r="Y78" s="2"/>
       <c r="Z78" s="2"/>
     </row>
-    <row r="79">
+    <row r="79" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="3">
-        <v>946.3684297</v>
+        <v>946.36842969999998</v>
       </c>
       <c r="B79" s="4">
-        <v>4.109343936</v>
+        <v>4.1093439360000001</v>
       </c>
       <c r="C79" s="5">
         <v>1.07</v>
@@ -2836,15 +2885,15 @@
       <c r="Y79" s="2"/>
       <c r="Z79" s="2"/>
     </row>
-    <row r="80">
+    <row r="80" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="3">
-        <v>951.8316619</v>
+        <v>951.83166189999997</v>
       </c>
       <c r="B80" s="4">
         <v>3.838966203</v>
       </c>
       <c r="C80" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D80" s="5"/>
       <c r="G80" s="2"/>
@@ -2868,12 +2917,12 @@
       <c r="Y80" s="2"/>
       <c r="Z80" s="2"/>
     </row>
-    <row r="81">
+    <row r="81" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="3">
-        <v>957.3264324</v>
+        <v>957.32643240000004</v>
       </c>
       <c r="B81" s="4">
-        <v>4.061630219</v>
+        <v>4.0616302190000004</v>
       </c>
       <c r="C81" s="5">
         <v>1.06</v>
@@ -2900,12 +2949,12 @@
       <c r="Y81" s="2"/>
       <c r="Z81" s="2"/>
     </row>
-    <row r="82">
+    <row r="82" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="3">
-        <v>968.4113178</v>
+        <v>968.41131780000001</v>
       </c>
       <c r="B82" s="4">
-        <v>4.109343936</v>
+        <v>4.1093439360000001</v>
       </c>
       <c r="C82" s="5">
         <v>1.07</v>
@@ -2932,12 +2981,12 @@
       <c r="Y82" s="2"/>
       <c r="Z82" s="2"/>
     </row>
-    <row r="83">
+    <row r="83" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="3">
-        <v>985.2797695</v>
+        <v>985.27976950000004</v>
       </c>
       <c r="B83" s="4">
-        <v>4.061630219</v>
+        <v>4.0616302190000004</v>
       </c>
       <c r="C83" s="5">
         <v>1.06</v>
@@ -2964,12 +3013,12 @@
       <c r="Y83" s="2"/>
       <c r="Z83" s="2"/>
     </row>
-    <row r="84">
+    <row r="84" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="3">
         <v>1000.520459</v>
       </c>
       <c r="B84" s="4">
-        <v>4.013916501</v>
+        <v>4.0139165009999997</v>
       </c>
       <c r="C84" s="5">
         <v>1.04</v>
@@ -2996,9 +3045,9 @@
       <c r="Y84" s="2"/>
       <c r="Z84" s="2"/>
     </row>
-    <row r="85">
+    <row r="85" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="3">
-        <v>1014.049327</v>
+        <v>1014.0493269999999</v>
       </c>
       <c r="B85" s="4">
         <v>4.029821074</v>
@@ -3028,7 +3077,7 @@
       <c r="Y85" s="2"/>
       <c r="Z85" s="2"/>
     </row>
-    <row r="86">
+    <row r="86" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="3">
         <v>1031.712732</v>
       </c>
@@ -3060,12 +3109,12 @@
       <c r="Y86" s="2"/>
       <c r="Z86" s="2"/>
     </row>
-    <row r="87">
+    <row r="87" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="3">
         <v>1049.683812</v>
       </c>
       <c r="B87" s="4">
-        <v>4.045725646</v>
+        <v>4.0457256460000002</v>
       </c>
       <c r="C87" s="5">
         <v>1.05</v>
@@ -3092,12 +3141,12 @@
       <c r="Y87" s="2"/>
       <c r="Z87" s="2"/>
     </row>
-    <row r="88">
+    <row r="88" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="3">
-        <v>1067.967923</v>
+        <v>1067.9679229999999</v>
       </c>
       <c r="B88" s="4">
-        <v>4.045725646</v>
+        <v>4.0457256460000002</v>
       </c>
       <c r="C88" s="5">
         <v>1.05</v>
@@ -3124,12 +3173,12 @@
       <c r="Y88" s="2"/>
       <c r="Z88" s="2"/>
     </row>
-    <row r="89">
+    <row r="89" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="3">
         <v>1086.57052</v>
       </c>
       <c r="B89" s="4">
-        <v>4.061630219</v>
+        <v>4.0616302190000004</v>
       </c>
       <c r="C89" s="5">
         <v>1.06</v>
@@ -3156,12 +3205,12 @@
       <c r="Y89" s="2"/>
       <c r="Z89" s="2"/>
     </row>
-    <row r="90">
+    <row r="90" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="3">
         <v>1107.620355</v>
       </c>
       <c r="B90" s="4">
-        <v>4.061630219</v>
+        <v>4.0616302190000004</v>
       </c>
       <c r="C90" s="5">
         <v>1.06</v>
@@ -3188,12 +3237,12 @@
       <c r="Y90" s="2"/>
       <c r="Z90" s="2"/>
     </row>
-    <row r="91">
+    <row r="91" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="3">
         <v>1131.246476</v>
       </c>
       <c r="B91" s="4">
-        <v>4.077534791</v>
+        <v>4.0775347909999997</v>
       </c>
       <c r="C91" s="5">
         <v>1.06</v>
@@ -3220,12 +3269,12 @@
       <c r="Y91" s="2"/>
       <c r="Z91" s="2"/>
     </row>
-    <row r="92">
+    <row r="92" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="3">
-        <v>1155.376556</v>
+        <v>1155.3765559999999</v>
       </c>
       <c r="B92" s="4">
-        <v>4.061630219</v>
+        <v>4.0616302190000004</v>
       </c>
       <c r="C92" s="5">
         <v>1.06</v>
@@ -3252,9 +3301,9 @@
       <c r="Y92" s="2"/>
       <c r="Z92" s="2"/>
     </row>
-    <row r="93">
+    <row r="93" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="3">
-        <v>1177.759351</v>
+        <v>1177.7593509999999</v>
       </c>
       <c r="B93" s="4">
         <v>4.029821074</v>
@@ -3284,9 +3333,9 @@
       <c r="Y93" s="2"/>
       <c r="Z93" s="2"/>
     </row>
-    <row r="94">
+    <row r="94" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="3">
-        <v>1198.27437</v>
+        <v>1198.2743700000001</v>
       </c>
       <c r="B94" s="4">
         <v>3.966202783</v>
@@ -3316,12 +3365,12 @@
       <c r="Y94" s="2"/>
       <c r="Z94" s="2"/>
     </row>
-    <row r="95">
+    <row r="95" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="3">
-        <v>1230.899186</v>
+        <v>1230.8991860000001</v>
       </c>
       <c r="B95" s="4">
-        <v>3.918489066</v>
+        <v>3.9184890659999998</v>
       </c>
       <c r="C95" s="5">
         <v>1.02</v>
@@ -3348,12 +3397,12 @@
       <c r="Y95" s="2"/>
       <c r="Z95" s="2"/>
     </row>
-    <row r="96">
+    <row r="96" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="3">
-        <v>1264.412262</v>
+        <v>1264.4122620000001</v>
       </c>
       <c r="B96" s="4">
-        <v>3.88667992</v>
+        <v>3.8866799200000002</v>
       </c>
       <c r="C96" s="5">
         <v>1.01</v>
@@ -3380,12 +3429,12 @@
       <c r="Y96" s="2"/>
       <c r="Z96" s="2"/>
     </row>
-    <row r="97">
+    <row r="97" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="3">
-        <v>1293.863052</v>
+        <v>1293.8630519999999</v>
       </c>
       <c r="B97" s="4">
-        <v>3.88667992</v>
+        <v>3.8866799200000002</v>
       </c>
       <c r="C97" s="5">
         <v>1.01</v>
@@ -3412,15 +3461,15 @@
       <c r="Y97" s="2"/>
       <c r="Z97" s="2"/>
     </row>
-    <row r="98">
+    <row r="98" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="3">
         <v>1321.461828</v>
       </c>
       <c r="B98" s="4">
-        <v>3.854870775</v>
+        <v>3.8548707750000002</v>
       </c>
       <c r="C98" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D98" s="5"/>
       <c r="G98" s="2"/>
@@ -3444,9 +3493,9 @@
       <c r="Y98" s="2"/>
       <c r="Z98" s="2"/>
     </row>
-    <row r="99">
+    <row r="99" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="3">
-        <v>1354.838521</v>
+        <v>1354.8385209999999</v>
       </c>
       <c r="B99" s="4">
         <v>3.807157058</v>
@@ -3476,12 +3525,12 @@
       <c r="Y99" s="2"/>
       <c r="Z99" s="2"/>
     </row>
-    <row r="100">
+    <row r="100" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A100" s="3">
         <v>1386.395526</v>
       </c>
       <c r="B100" s="4">
-        <v>3.75944334</v>
+        <v>3.7594433399999998</v>
       </c>
       <c r="C100" s="5">
         <v>0.98</v>
@@ -3508,12 +3557,12 @@
       <c r="Y100" s="2"/>
       <c r="Z100" s="2"/>
     </row>
-    <row r="101">
+    <row r="101" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A101" s="3">
-        <v>1421.412275</v>
+        <v>1421.4122749999999</v>
       </c>
       <c r="B101" s="4">
-        <v>3.69582505</v>
+        <v>3.6958250499999998</v>
       </c>
       <c r="C101" s="5">
         <v>0.96</v>
@@ -3540,9 +3589,9 @@
       <c r="Y101" s="2"/>
       <c r="Z101" s="2"/>
     </row>
-    <row r="102">
+    <row r="102" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A102" s="3">
-        <v>1451.731742</v>
+        <v>1451.7317419999999</v>
       </c>
       <c r="B102" s="4">
         <v>3.679920477</v>
@@ -3572,7 +3621,7 @@
       <c r="Y102" s="2"/>
       <c r="Z102" s="2"/>
     </row>
-    <row r="103">
+    <row r="103" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A103" s="3">
         <v>1482.69794</v>
       </c>
@@ -3604,12 +3653,12 @@
       <c r="Y103" s="2"/>
       <c r="Z103" s="2"/>
     </row>
-    <row r="104">
+    <row r="104" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A104" s="3">
-        <v>1517.233057</v>
+        <v>1517.2330569999999</v>
       </c>
       <c r="B104" s="4">
-        <v>3.600397614</v>
+        <v>3.6003976139999998</v>
       </c>
       <c r="C104" s="5">
         <v>0.94</v>
@@ -3636,9 +3685,9 @@
       <c r="Y104" s="2"/>
       <c r="Z104" s="2"/>
     </row>
-    <row r="105">
+    <row r="105" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A105" s="3">
-        <v>1552.572569</v>
+        <v>1552.5725689999999</v>
       </c>
       <c r="B105" s="4">
         <v>3.520874751</v>
@@ -3668,12 +3717,12 @@
       <c r="Y105" s="2"/>
       <c r="Z105" s="2"/>
     </row>
-    <row r="106">
+    <row r="106" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A106" s="3">
-        <v>1591.786518</v>
+        <v>1591.7865179999999</v>
       </c>
       <c r="B106" s="4">
-        <v>3.473161034</v>
+        <v>3.4731610339999999</v>
       </c>
       <c r="C106" s="5">
         <v>0.9</v>
@@ -3700,12 +3749,12 @@
       <c r="Y106" s="2"/>
       <c r="Z106" s="2"/>
     </row>
-    <row r="107">
+    <row r="107" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A107" s="3">
         <v>1619.513346</v>
       </c>
       <c r="B107" s="4">
-        <v>3.441351889</v>
+        <v>3.4413518889999999</v>
       </c>
       <c r="C107" s="5">
         <v>0.89</v>
@@ -3732,12 +3781,12 @@
       <c r="Y107" s="2"/>
       <c r="Z107" s="2"/>
     </row>
-    <row r="108">
+    <row r="108" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A108" s="3">
-        <v>1676.42431</v>
+        <v>1676.4243100000001</v>
       </c>
       <c r="B108" s="4">
-        <v>3.345924453</v>
+        <v>3.3459244529999999</v>
       </c>
       <c r="C108" s="5">
         <v>0.87</v>
@@ -3764,12 +3813,12 @@
       <c r="Y108" s="2"/>
       <c r="Z108" s="2"/>
     </row>
-    <row r="109">
+    <row r="109" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A109" s="3">
         <v>1712.183317</v>
       </c>
       <c r="B109" s="4">
-        <v>3.314115308</v>
+        <v>3.3141153079999999</v>
       </c>
       <c r="C109" s="5">
         <v>0.86</v>
@@ -3796,12 +3845,12 @@
       <c r="Y109" s="2"/>
       <c r="Z109" s="2"/>
     </row>
-    <row r="110">
+    <row r="110" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A110" s="3">
-        <v>1758.800075</v>
+        <v>1758.8000750000001</v>
       </c>
       <c r="B110" s="4">
-        <v>3.298210736</v>
+        <v>3.2982107360000001</v>
       </c>
       <c r="C110" s="5">
         <v>0.86</v>
@@ -3828,12 +3877,12 @@
       <c r="Y110" s="2"/>
       <c r="Z110" s="2"/>
     </row>
-    <row r="111">
+    <row r="111" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A111" s="3">
         <v>1799.766185</v>
       </c>
       <c r="B111" s="4">
-        <v>3.282306163</v>
+        <v>3.2823061629999999</v>
       </c>
       <c r="C111" s="5">
         <v>0.85</v>
@@ -3860,12 +3909,12 @@
       <c r="Y111" s="2"/>
       <c r="Z111" s="2"/>
     </row>
-    <row r="112">
+    <row r="112" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A112" s="3">
-        <v>1845.223603</v>
+        <v>1845.2236029999999</v>
       </c>
       <c r="B112" s="4">
-        <v>3.250497018</v>
+        <v>3.2504970179999999</v>
       </c>
       <c r="C112" s="5">
         <v>0.85</v>
@@ -3892,12 +3941,12 @@
       <c r="Y112" s="2"/>
       <c r="Z112" s="2"/>
     </row>
-    <row r="113">
+    <row r="113" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A113" s="3">
-        <v>1888.202696</v>
+        <v>1888.2026960000001</v>
       </c>
       <c r="B113" s="4">
-        <v>3.2027833</v>
+        <v>3.2027833000000001</v>
       </c>
       <c r="C113" s="5">
         <v>0.83</v>
@@ -3924,12 +3973,12 @@
       <c r="Y113" s="2"/>
       <c r="Z113" s="2"/>
     </row>
-    <row r="114">
+    <row r="114" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A114" s="3">
-        <v>1924.782333</v>
+        <v>1924.7823330000001</v>
       </c>
       <c r="B114" s="4">
-        <v>3.170974155</v>
+        <v>3.1709741550000001</v>
       </c>
       <c r="C114" s="5">
         <v>0.82</v>
@@ -3956,12 +4005,12 @@
       <c r="Y114" s="2"/>
       <c r="Z114" s="2"/>
     </row>
-    <row r="115">
+    <row r="115" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A115" s="3">
-        <v>1962.070617</v>
+        <v>1962.0706170000001</v>
       </c>
       <c r="B115" s="4">
-        <v>3.13916501</v>
+        <v>3.1391650100000001</v>
       </c>
       <c r="C115" s="5">
         <v>0.82</v>
@@ -3988,12 +4037,12 @@
       <c r="Y115" s="2"/>
       <c r="Z115" s="2"/>
     </row>
-    <row r="116">
+    <row r="116" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A116" s="3">
         <v>2003.922609</v>
       </c>
       <c r="B116" s="4">
-        <v>3.13916501</v>
+        <v>3.1391650100000001</v>
       </c>
       <c r="C116" s="5">
         <v>0.82</v>
@@ -4020,12 +4069,12 @@
       <c r="Y116" s="2"/>
       <c r="Z116" s="2"/>
     </row>
-    <row r="117">
+    <row r="117" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A117" s="3">
-        <v>2054.536488</v>
+        <v>2054.5364880000002</v>
       </c>
       <c r="B117" s="4">
-        <v>3.07554672</v>
+        <v>3.0755467200000002</v>
       </c>
       <c r="C117" s="5">
         <v>0.8</v>
@@ -4052,12 +4101,12 @@
       <c r="Y117" s="2"/>
       <c r="Z117" s="2"/>
     </row>
-    <row r="118">
+    <row r="118" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A118" s="3">
-        <v>2122.657752</v>
+        <v>2122.6577520000001</v>
       </c>
       <c r="B118" s="4">
-        <v>3.011928429</v>
+        <v>3.0119284290000001</v>
       </c>
       <c r="C118" s="5">
         <v>0.78</v>
@@ -4084,9 +4133,9 @@
       <c r="Y118" s="2"/>
       <c r="Z118" s="2"/>
     </row>
-    <row r="119">
+    <row r="119" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A119" s="3">
-        <v>2176.270572</v>
+        <v>2176.2705719999999</v>
       </c>
       <c r="B119" s="4">
         <v>2.996023857</v>
@@ -4116,12 +4165,12 @@
       <c r="Y119" s="2"/>
       <c r="Z119" s="2"/>
     </row>
-    <row r="120">
+    <row r="120" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A120" s="3">
-        <v>2218.430869</v>
+        <v>2218.4308689999998</v>
       </c>
       <c r="B120" s="4">
-        <v>2.980119284</v>
+        <v>2.9801192840000001</v>
       </c>
       <c r="C120" s="5">
         <v>0.77</v>
@@ -4148,12 +4197,12 @@
       <c r="Y120" s="2"/>
       <c r="Z120" s="2"/>
     </row>
-    <row r="121">
+    <row r="121" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A121" s="3">
-        <v>2265.75116</v>
+        <v>2265.7511599999998</v>
       </c>
       <c r="B121" s="4">
-        <v>2.948310139</v>
+        <v>2.9483101390000002</v>
       </c>
       <c r="C121" s="5">
         <v>0.77</v>
@@ -4180,12 +4229,12 @@
       <c r="Y121" s="2"/>
       <c r="Z121" s="2"/>
     </row>
-    <row r="122">
+    <row r="122" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="3">
-        <v>2318.525214</v>
+        <v>2318.5252139999998</v>
       </c>
       <c r="B122" s="4">
-        <v>2.884691849</v>
+        <v>2.8846918490000002</v>
       </c>
       <c r="C122" s="5">
         <v>0.75</v>
@@ -4212,12 +4261,12 @@
       <c r="Y122" s="2"/>
       <c r="Z122" s="2"/>
     </row>
-    <row r="123">
+    <row r="123" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A123" s="3">
-        <v>2367.98057</v>
+        <v>2367.9805700000002</v>
       </c>
       <c r="B123" s="4">
-        <v>2.868787276</v>
+        <v>2.8687872759999999</v>
       </c>
       <c r="C123" s="5">
         <v>0.75</v>
@@ -4244,9 +4293,9 @@
       <c r="Y123" s="2"/>
       <c r="Z123" s="2"/>
     </row>
-    <row r="124">
+    <row r="124" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A124" s="3">
-        <v>2432.452391</v>
+        <v>2432.4523909999998</v>
       </c>
       <c r="B124" s="4">
         <v>2.836978131</v>
@@ -4276,12 +4325,12 @@
       <c r="Y124" s="2"/>
       <c r="Z124" s="2"/>
     </row>
-    <row r="125">
+    <row r="125" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A125" s="3">
-        <v>2489.109264</v>
+        <v>2489.1092640000002</v>
       </c>
       <c r="B125" s="4">
-        <v>2.789264414</v>
+        <v>2.7892644139999998</v>
       </c>
       <c r="C125" s="5">
         <v>0.73</v>
@@ -4308,9 +4357,9 @@
       <c r="Y125" s="2"/>
       <c r="Z125" s="2"/>
     </row>
-    <row r="126">
+    <row r="126" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A126" s="3">
-        <v>2551.977697</v>
+        <v>2551.9776969999998</v>
       </c>
       <c r="B126" s="4">
         <v>2.741550696</v>
@@ -4340,7 +4389,7 @@
       <c r="Y126" s="2"/>
       <c r="Z126" s="2"/>
     </row>
-    <row r="127">
+    <row r="127" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A127" s="3"/>
       <c r="B127" s="4"/>
       <c r="C127" s="5"/>
@@ -4366,7 +4415,7 @@
       <c r="Y127" s="2"/>
       <c r="Z127" s="2"/>
     </row>
-    <row r="128">
+    <row r="128" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A128" s="3"/>
       <c r="B128" s="4"/>
       <c r="C128" s="5"/>
@@ -4392,7 +4441,7 @@
       <c r="Y128" s="2"/>
       <c r="Z128" s="2"/>
     </row>
-    <row r="129">
+    <row r="129" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A129" s="3"/>
       <c r="B129" s="4"/>
       <c r="C129" s="5"/>
@@ -4418,7 +4467,7 @@
       <c r="Y129" s="2"/>
       <c r="Z129" s="2"/>
     </row>
-    <row r="130">
+    <row r="130" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A130" s="3"/>
       <c r="B130" s="4"/>
       <c r="C130" s="5"/>
@@ -4444,7 +4493,7 @@
       <c r="Y130" s="2"/>
       <c r="Z130" s="2"/>
     </row>
-    <row r="131">
+    <row r="131" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A131" s="3"/>
       <c r="B131" s="4"/>
       <c r="C131" s="5"/>
@@ -4470,7 +4519,7 @@
       <c r="Y131" s="2"/>
       <c r="Z131" s="2"/>
     </row>
-    <row r="132">
+    <row r="132" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A132" s="3"/>
       <c r="B132" s="4"/>
       <c r="C132" s="5"/>
@@ -4496,7 +4545,7 @@
       <c r="Y132" s="2"/>
       <c r="Z132" s="2"/>
     </row>
-    <row r="133">
+    <row r="133" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A133" s="3"/>
       <c r="B133" s="4"/>
       <c r="C133" s="5"/>
@@ -4522,7 +4571,7 @@
       <c r="Y133" s="2"/>
       <c r="Z133" s="2"/>
     </row>
-    <row r="134">
+    <row r="134" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A134" s="3"/>
       <c r="B134" s="4"/>
       <c r="C134" s="5"/>
@@ -4548,7 +4597,7 @@
       <c r="Y134" s="2"/>
       <c r="Z134" s="2"/>
     </row>
-    <row r="135">
+    <row r="135" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A135" s="3"/>
       <c r="B135" s="4"/>
       <c r="C135" s="5"/>
@@ -4574,7 +4623,7 @@
       <c r="Y135" s="2"/>
       <c r="Z135" s="2"/>
     </row>
-    <row r="136">
+    <row r="136" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A136" s="3"/>
       <c r="B136" s="4"/>
       <c r="C136" s="5"/>
@@ -4600,7 +4649,7 @@
       <c r="Y136" s="2"/>
       <c r="Z136" s="2"/>
     </row>
-    <row r="137">
+    <row r="137" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A137" s="3"/>
       <c r="B137" s="4"/>
       <c r="C137" s="5"/>
@@ -4626,7 +4675,7 @@
       <c r="Y137" s="2"/>
       <c r="Z137" s="2"/>
     </row>
-    <row r="138">
+    <row r="138" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A138" s="3"/>
       <c r="B138" s="4"/>
       <c r="C138" s="5"/>
@@ -4652,7 +4701,7 @@
       <c r="Y138" s="2"/>
       <c r="Z138" s="2"/>
     </row>
-    <row r="139">
+    <row r="139" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A139" s="3"/>
       <c r="B139" s="4"/>
       <c r="C139" s="5"/>
@@ -4678,7 +4727,7 @@
       <c r="Y139" s="2"/>
       <c r="Z139" s="2"/>
     </row>
-    <row r="140">
+    <row r="140" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A140" s="3"/>
       <c r="B140" s="4"/>
       <c r="C140" s="5"/>
@@ -4704,7 +4753,7 @@
       <c r="Y140" s="2"/>
       <c r="Z140" s="2"/>
     </row>
-    <row r="141">
+    <row r="141" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A141" s="3"/>
       <c r="B141" s="4"/>
       <c r="C141" s="5"/>
@@ -4730,7 +4779,7 @@
       <c r="Y141" s="2"/>
       <c r="Z141" s="2"/>
     </row>
-    <row r="142">
+    <row r="142" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A142" s="3"/>
       <c r="B142" s="4"/>
       <c r="C142" s="5"/>
@@ -4756,7 +4805,7 @@
       <c r="Y142" s="2"/>
       <c r="Z142" s="2"/>
     </row>
-    <row r="143">
+    <row r="143" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A143" s="3"/>
       <c r="B143" s="4"/>
       <c r="C143" s="5"/>
@@ -4782,7 +4831,7 @@
       <c r="Y143" s="2"/>
       <c r="Z143" s="2"/>
     </row>
-    <row r="144">
+    <row r="144" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A144" s="3"/>
       <c r="B144" s="4"/>
       <c r="C144" s="5"/>
@@ -4808,7 +4857,7 @@
       <c r="Y144" s="2"/>
       <c r="Z144" s="2"/>
     </row>
-    <row r="145">
+    <row r="145" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A145" s="3"/>
       <c r="B145" s="4"/>
       <c r="C145" s="5"/>
@@ -4834,7 +4883,7 @@
       <c r="Y145" s="2"/>
       <c r="Z145" s="2"/>
     </row>
-    <row r="146">
+    <row r="146" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A146" s="3"/>
       <c r="B146" s="4"/>
       <c r="C146" s="5"/>
@@ -4860,7 +4909,7 @@
       <c r="Y146" s="2"/>
       <c r="Z146" s="2"/>
     </row>
-    <row r="147">
+    <row r="147" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A147" s="3"/>
       <c r="B147" s="4"/>
       <c r="C147" s="5"/>
@@ -4886,7 +4935,7 @@
       <c r="Y147" s="2"/>
       <c r="Z147" s="2"/>
     </row>
-    <row r="148">
+    <row r="148" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A148" s="3"/>
       <c r="B148" s="4"/>
       <c r="C148" s="5"/>
@@ -4912,7 +4961,7 @@
       <c r="Y148" s="2"/>
       <c r="Z148" s="2"/>
     </row>
-    <row r="149">
+    <row r="149" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A149" s="3"/>
       <c r="B149" s="4"/>
       <c r="C149" s="5"/>
@@ -4938,7 +4987,7 @@
       <c r="Y149" s="2"/>
       <c r="Z149" s="2"/>
     </row>
-    <row r="150">
+    <row r="150" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A150" s="3"/>
       <c r="B150" s="4"/>
       <c r="C150" s="5"/>
@@ -4964,7 +5013,7 @@
       <c r="Y150" s="2"/>
       <c r="Z150" s="2"/>
     </row>
-    <row r="151">
+    <row r="151" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A151" s="3"/>
       <c r="B151" s="4"/>
       <c r="C151" s="5"/>
@@ -4990,7 +5039,7 @@
       <c r="Y151" s="2"/>
       <c r="Z151" s="2"/>
     </row>
-    <row r="152">
+    <row r="152" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A152" s="3"/>
       <c r="B152" s="4"/>
       <c r="C152" s="5"/>
@@ -5016,7 +5065,7 @@
       <c r="Y152" s="2"/>
       <c r="Z152" s="2"/>
     </row>
-    <row r="153">
+    <row r="153" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A153" s="3"/>
       <c r="B153" s="4"/>
       <c r="C153" s="5"/>
@@ -5042,7 +5091,7 @@
       <c r="Y153" s="2"/>
       <c r="Z153" s="2"/>
     </row>
-    <row r="154">
+    <row r="154" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A154" s="3"/>
       <c r="B154" s="4"/>
       <c r="C154" s="5"/>
@@ -5068,7 +5117,7 @@
       <c r="Y154" s="2"/>
       <c r="Z154" s="2"/>
     </row>
-    <row r="155">
+    <row r="155" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A155" s="3"/>
       <c r="B155" s="4"/>
       <c r="C155" s="5"/>
@@ -5094,7 +5143,7 @@
       <c r="Y155" s="2"/>
       <c r="Z155" s="2"/>
     </row>
-    <row r="156">
+    <row r="156" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A156" s="3"/>
       <c r="B156" s="4"/>
       <c r="C156" s="5"/>
@@ -5120,7 +5169,7 @@
       <c r="Y156" s="2"/>
       <c r="Z156" s="2"/>
     </row>
-    <row r="157">
+    <row r="157" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A157" s="3"/>
       <c r="B157" s="4"/>
       <c r="C157" s="5"/>
@@ -5146,7 +5195,7 @@
       <c r="Y157" s="2"/>
       <c r="Z157" s="2"/>
     </row>
-    <row r="158">
+    <row r="158" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A158" s="3"/>
       <c r="B158" s="4"/>
       <c r="C158" s="5"/>
@@ -5172,7 +5221,7 @@
       <c r="Y158" s="2"/>
       <c r="Z158" s="2"/>
     </row>
-    <row r="159">
+    <row r="159" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A159" s="3"/>
       <c r="B159" s="4"/>
       <c r="C159" s="5"/>
@@ -5198,7 +5247,7 @@
       <c r="Y159" s="2"/>
       <c r="Z159" s="2"/>
     </row>
-    <row r="160">
+    <row r="160" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A160" s="3"/>
       <c r="B160" s="4"/>
       <c r="C160" s="5"/>
@@ -5224,7 +5273,7 @@
       <c r="Y160" s="2"/>
       <c r="Z160" s="2"/>
     </row>
-    <row r="161">
+    <row r="161" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A161" s="3"/>
       <c r="B161" s="4"/>
       <c r="C161" s="5"/>
@@ -5250,7 +5299,7 @@
       <c r="Y161" s="2"/>
       <c r="Z161" s="2"/>
     </row>
-    <row r="162">
+    <row r="162" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A162" s="3"/>
       <c r="B162" s="4"/>
       <c r="C162" s="5"/>
@@ -5276,7 +5325,7 @@
       <c r="Y162" s="2"/>
       <c r="Z162" s="2"/>
     </row>
-    <row r="163">
+    <row r="163" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A163" s="3"/>
       <c r="B163" s="4"/>
       <c r="C163" s="5"/>
@@ -5302,7 +5351,7 @@
       <c r="Y163" s="2"/>
       <c r="Z163" s="2"/>
     </row>
-    <row r="164">
+    <row r="164" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A164" s="3"/>
       <c r="B164" s="4"/>
       <c r="C164" s="5"/>
@@ -5328,7 +5377,7 @@
       <c r="Y164" s="2"/>
       <c r="Z164" s="2"/>
     </row>
-    <row r="165">
+    <row r="165" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A165" s="3"/>
       <c r="B165" s="4"/>
       <c r="C165" s="5"/>
@@ -5354,7 +5403,7 @@
       <c r="Y165" s="2"/>
       <c r="Z165" s="2"/>
     </row>
-    <row r="166">
+    <row r="166" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A166" s="3"/>
       <c r="B166" s="4"/>
       <c r="C166" s="5"/>
@@ -5380,7 +5429,7 @@
       <c r="Y166" s="2"/>
       <c r="Z166" s="2"/>
     </row>
-    <row r="167">
+    <row r="167" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A167" s="3"/>
       <c r="B167" s="4"/>
       <c r="C167" s="5"/>
@@ -5406,7 +5455,7 @@
       <c r="Y167" s="2"/>
       <c r="Z167" s="2"/>
     </row>
-    <row r="168">
+    <row r="168" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A168" s="3"/>
       <c r="B168" s="4"/>
       <c r="C168" s="5"/>
@@ -5432,7 +5481,7 @@
       <c r="Y168" s="2"/>
       <c r="Z168" s="2"/>
     </row>
-    <row r="169">
+    <row r="169" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A169" s="3"/>
       <c r="B169" s="4"/>
       <c r="C169" s="5"/>
@@ -5458,7 +5507,7 @@
       <c r="Y169" s="2"/>
       <c r="Z169" s="2"/>
     </row>
-    <row r="170">
+    <row r="170" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A170" s="3"/>
       <c r="B170" s="4"/>
       <c r="C170" s="5"/>
@@ -5484,7 +5533,7 @@
       <c r="Y170" s="2"/>
       <c r="Z170" s="2"/>
     </row>
-    <row r="171">
+    <row r="171" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A171" s="3"/>
       <c r="B171" s="4"/>
       <c r="C171" s="5"/>
@@ -5510,7 +5559,7 @@
       <c r="Y171" s="2"/>
       <c r="Z171" s="2"/>
     </row>
-    <row r="172">
+    <row r="172" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A172" s="3"/>
       <c r="B172" s="4"/>
       <c r="C172" s="5"/>
@@ -5536,7 +5585,7 @@
       <c r="Y172" s="2"/>
       <c r="Z172" s="2"/>
     </row>
-    <row r="173">
+    <row r="173" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A173" s="3"/>
       <c r="B173" s="4"/>
       <c r="C173" s="5"/>
@@ -5562,7 +5611,7 @@
       <c r="Y173" s="2"/>
       <c r="Z173" s="2"/>
     </row>
-    <row r="174">
+    <row r="174" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A174" s="3"/>
       <c r="B174" s="4"/>
       <c r="C174" s="5"/>
@@ -5588,7 +5637,7 @@
       <c r="Y174" s="2"/>
       <c r="Z174" s="2"/>
     </row>
-    <row r="175">
+    <row r="175" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A175" s="3"/>
       <c r="B175" s="4"/>
       <c r="C175" s="5"/>
@@ -5614,7 +5663,7 @@
       <c r="Y175" s="2"/>
       <c r="Z175" s="2"/>
     </row>
-    <row r="176">
+    <row r="176" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A176" s="3"/>
       <c r="B176" s="4"/>
       <c r="C176" s="5"/>
@@ -5640,7 +5689,7 @@
       <c r="Y176" s="2"/>
       <c r="Z176" s="2"/>
     </row>
-    <row r="177">
+    <row r="177" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A177" s="3"/>
       <c r="B177" s="4"/>
       <c r="C177" s="5"/>
@@ -5666,7 +5715,7 @@
       <c r="Y177" s="2"/>
       <c r="Z177" s="2"/>
     </row>
-    <row r="178">
+    <row r="178" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A178" s="3"/>
       <c r="B178" s="4"/>
       <c r="C178" s="5"/>
@@ -5692,7 +5741,7 @@
       <c r="Y178" s="2"/>
       <c r="Z178" s="2"/>
     </row>
-    <row r="179">
+    <row r="179" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A179" s="3"/>
       <c r="B179" s="4"/>
       <c r="C179" s="5"/>
@@ -5718,7 +5767,7 @@
       <c r="Y179" s="2"/>
       <c r="Z179" s="2"/>
     </row>
-    <row r="180">
+    <row r="180" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A180" s="3"/>
       <c r="B180" s="4"/>
       <c r="C180" s="5"/>
@@ -5744,7 +5793,7 @@
       <c r="Y180" s="2"/>
       <c r="Z180" s="2"/>
     </row>
-    <row r="181">
+    <row r="181" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A181" s="3"/>
       <c r="B181" s="4"/>
       <c r="C181" s="5"/>
@@ -5770,7 +5819,7 @@
       <c r="Y181" s="2"/>
       <c r="Z181" s="2"/>
     </row>
-    <row r="182">
+    <row r="182" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A182" s="3"/>
       <c r="B182" s="4"/>
       <c r="C182" s="5"/>
@@ -5796,7 +5845,7 @@
       <c r="Y182" s="2"/>
       <c r="Z182" s="2"/>
     </row>
-    <row r="183">
+    <row r="183" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A183" s="3"/>
       <c r="B183" s="4"/>
       <c r="C183" s="5"/>
@@ -5822,7 +5871,7 @@
       <c r="Y183" s="2"/>
       <c r="Z183" s="2"/>
     </row>
-    <row r="184">
+    <row r="184" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A184" s="3"/>
       <c r="B184" s="4"/>
       <c r="C184" s="5"/>
@@ -5848,7 +5897,7 @@
       <c r="Y184" s="2"/>
       <c r="Z184" s="2"/>
     </row>
-    <row r="185">
+    <row r="185" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A185" s="3"/>
       <c r="B185" s="4"/>
       <c r="C185" s="5"/>
@@ -5874,7 +5923,7 @@
       <c r="Y185" s="2"/>
       <c r="Z185" s="2"/>
     </row>
-    <row r="186">
+    <row r="186" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A186" s="3"/>
       <c r="B186" s="4"/>
       <c r="C186" s="5"/>
@@ -5900,7 +5949,7 @@
       <c r="Y186" s="2"/>
       <c r="Z186" s="2"/>
     </row>
-    <row r="187">
+    <row r="187" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A187" s="3"/>
       <c r="B187" s="4"/>
       <c r="C187" s="5"/>
@@ -5926,7 +5975,7 @@
       <c r="Y187" s="2"/>
       <c r="Z187" s="2"/>
     </row>
-    <row r="188">
+    <row r="188" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A188" s="3"/>
       <c r="B188" s="4"/>
       <c r="C188" s="5"/>
@@ -5952,7 +6001,7 @@
       <c r="Y188" s="2"/>
       <c r="Z188" s="2"/>
     </row>
-    <row r="189">
+    <row r="189" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A189" s="3"/>
       <c r="B189" s="4"/>
       <c r="C189" s="5"/>
@@ -5978,7 +6027,7 @@
       <c r="Y189" s="2"/>
       <c r="Z189" s="2"/>
     </row>
-    <row r="190">
+    <row r="190" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A190" s="3"/>
       <c r="B190" s="4"/>
       <c r="C190" s="5"/>
@@ -6004,7 +6053,7 @@
       <c r="Y190" s="2"/>
       <c r="Z190" s="2"/>
     </row>
-    <row r="191">
+    <row r="191" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A191" s="3"/>
       <c r="B191" s="4"/>
       <c r="C191" s="5"/>
@@ -6030,7 +6079,7 @@
       <c r="Y191" s="2"/>
       <c r="Z191" s="2"/>
     </row>
-    <row r="192">
+    <row r="192" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A192" s="3"/>
       <c r="B192" s="4"/>
       <c r="C192" s="5"/>
@@ -6056,7 +6105,7 @@
       <c r="Y192" s="2"/>
       <c r="Z192" s="2"/>
     </row>
-    <row r="193">
+    <row r="193" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A193" s="3"/>
       <c r="B193" s="4"/>
       <c r="C193" s="5"/>
@@ -6082,7 +6131,7 @@
       <c r="Y193" s="2"/>
       <c r="Z193" s="2"/>
     </row>
-    <row r="194">
+    <row r="194" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A194" s="3"/>
       <c r="B194" s="4"/>
       <c r="C194" s="5"/>
@@ -6108,7 +6157,7 @@
       <c r="Y194" s="2"/>
       <c r="Z194" s="2"/>
     </row>
-    <row r="195">
+    <row r="195" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A195" s="3"/>
       <c r="B195" s="4"/>
       <c r="C195" s="5"/>
@@ -6134,7 +6183,7 @@
       <c r="Y195" s="2"/>
       <c r="Z195" s="2"/>
     </row>
-    <row r="196">
+    <row r="196" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A196" s="3"/>
       <c r="B196" s="4"/>
       <c r="C196" s="5"/>
@@ -6160,7 +6209,7 @@
       <c r="Y196" s="2"/>
       <c r="Z196" s="2"/>
     </row>
-    <row r="197">
+    <row r="197" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A197" s="3"/>
       <c r="B197" s="4"/>
       <c r="C197" s="5"/>
@@ -6186,7 +6235,7 @@
       <c r="Y197" s="2"/>
       <c r="Z197" s="2"/>
     </row>
-    <row r="198">
+    <row r="198" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A198" s="3"/>
       <c r="B198" s="4"/>
       <c r="C198" s="5"/>
@@ -6212,7 +6261,7 @@
       <c r="Y198" s="2"/>
       <c r="Z198" s="2"/>
     </row>
-    <row r="199">
+    <row r="199" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A199" s="3"/>
       <c r="B199" s="4"/>
       <c r="C199" s="5"/>
@@ -6238,7 +6287,7 @@
       <c r="Y199" s="2"/>
       <c r="Z199" s="2"/>
     </row>
-    <row r="200">
+    <row r="200" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A200" s="3"/>
       <c r="B200" s="4"/>
       <c r="C200" s="5"/>
@@ -6264,7 +6313,7 @@
       <c r="Y200" s="2"/>
       <c r="Z200" s="2"/>
     </row>
-    <row r="201">
+    <row r="201" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A201" s="3"/>
       <c r="B201" s="4"/>
       <c r="C201" s="5"/>
@@ -6290,7 +6339,7 @@
       <c r="Y201" s="2"/>
       <c r="Z201" s="2"/>
     </row>
-    <row r="202">
+    <row r="202" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A202" s="3"/>
       <c r="B202" s="4"/>
       <c r="C202" s="5"/>
@@ -6316,7 +6365,7 @@
       <c r="Y202" s="2"/>
       <c r="Z202" s="2"/>
     </row>
-    <row r="203">
+    <row r="203" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A203" s="3"/>
       <c r="B203" s="4"/>
       <c r="C203" s="5"/>
@@ -6342,7 +6391,7 @@
       <c r="Y203" s="2"/>
       <c r="Z203" s="2"/>
     </row>
-    <row r="204">
+    <row r="204" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A204" s="3"/>
       <c r="B204" s="4"/>
       <c r="C204" s="5"/>
@@ -6368,7 +6417,7 @@
       <c r="Y204" s="2"/>
       <c r="Z204" s="2"/>
     </row>
-    <row r="205">
+    <row r="205" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A205" s="3"/>
       <c r="B205" s="4"/>
       <c r="C205" s="5"/>
@@ -6394,7 +6443,7 @@
       <c r="Y205" s="2"/>
       <c r="Z205" s="2"/>
     </row>
-    <row r="206">
+    <row r="206" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A206" s="3"/>
       <c r="B206" s="4"/>
       <c r="C206" s="5"/>
@@ -6420,7 +6469,7 @@
       <c r="Y206" s="2"/>
       <c r="Z206" s="2"/>
     </row>
-    <row r="207">
+    <row r="207" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A207" s="3"/>
       <c r="B207" s="4"/>
       <c r="C207" s="5"/>
@@ -6446,7 +6495,7 @@
       <c r="Y207" s="2"/>
       <c r="Z207" s="2"/>
     </row>
-    <row r="208">
+    <row r="208" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A208" s="3"/>
       <c r="B208" s="4"/>
       <c r="C208" s="5"/>
@@ -6472,7 +6521,7 @@
       <c r="Y208" s="2"/>
       <c r="Z208" s="2"/>
     </row>
-    <row r="209">
+    <row r="209" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A209" s="3"/>
       <c r="B209" s="4"/>
       <c r="C209" s="5"/>
@@ -6498,7 +6547,7 @@
       <c r="Y209" s="2"/>
       <c r="Z209" s="2"/>
     </row>
-    <row r="210">
+    <row r="210" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A210" s="3"/>
       <c r="B210" s="4"/>
       <c r="C210" s="5"/>
@@ -6524,7 +6573,7 @@
       <c r="Y210" s="2"/>
       <c r="Z210" s="2"/>
     </row>
-    <row r="211">
+    <row r="211" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A211" s="3"/>
       <c r="B211" s="4"/>
       <c r="C211" s="5"/>
@@ -6550,7 +6599,7 @@
       <c r="Y211" s="2"/>
       <c r="Z211" s="2"/>
     </row>
-    <row r="212">
+    <row r="212" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A212" s="3"/>
       <c r="B212" s="4"/>
       <c r="C212" s="5"/>
@@ -6576,7 +6625,7 @@
       <c r="Y212" s="2"/>
       <c r="Z212" s="2"/>
     </row>
-    <row r="213">
+    <row r="213" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A213" s="3"/>
       <c r="B213" s="4"/>
       <c r="C213" s="5"/>
@@ -6602,7 +6651,7 @@
       <c r="Y213" s="2"/>
       <c r="Z213" s="2"/>
     </row>
-    <row r="214">
+    <row r="214" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A214" s="3"/>
       <c r="B214" s="4"/>
       <c r="C214" s="5"/>
@@ -6628,7 +6677,7 @@
       <c r="Y214" s="2"/>
       <c r="Z214" s="2"/>
     </row>
-    <row r="215">
+    <row r="215" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A215" s="3"/>
       <c r="B215" s="4"/>
       <c r="C215" s="5"/>
@@ -6654,7 +6703,7 @@
       <c r="Y215" s="2"/>
       <c r="Z215" s="2"/>
     </row>
-    <row r="216">
+    <row r="216" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A216" s="3"/>
       <c r="B216" s="4"/>
       <c r="C216" s="5"/>
@@ -6680,7 +6729,7 @@
       <c r="Y216" s="2"/>
       <c r="Z216" s="2"/>
     </row>
-    <row r="217">
+    <row r="217" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A217" s="3"/>
       <c r="B217" s="4"/>
       <c r="C217" s="5"/>
@@ -6706,7 +6755,7 @@
       <c r="Y217" s="2"/>
       <c r="Z217" s="2"/>
     </row>
-    <row r="218">
+    <row r="218" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A218" s="3"/>
       <c r="B218" s="4"/>
       <c r="C218" s="5"/>
@@ -6732,7 +6781,7 @@
       <c r="Y218" s="2"/>
       <c r="Z218" s="2"/>
     </row>
-    <row r="219">
+    <row r="219" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A219" s="3"/>
       <c r="B219" s="4"/>
       <c r="C219" s="5"/>
@@ -6758,7 +6807,7 @@
       <c r="Y219" s="2"/>
       <c r="Z219" s="2"/>
     </row>
-    <row r="220">
+    <row r="220" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A220" s="3"/>
       <c r="B220" s="4"/>
       <c r="C220" s="5"/>
@@ -6784,7 +6833,7 @@
       <c r="Y220" s="2"/>
       <c r="Z220" s="2"/>
     </row>
-    <row r="221">
+    <row r="221" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A221" s="3"/>
       <c r="B221" s="4"/>
       <c r="C221" s="5"/>
@@ -6810,7 +6859,7 @@
       <c r="Y221" s="2"/>
       <c r="Z221" s="2"/>
     </row>
-    <row r="222">
+    <row r="222" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A222" s="3"/>
       <c r="B222" s="4"/>
       <c r="C222" s="5"/>
@@ -6836,7 +6885,7 @@
       <c r="Y222" s="2"/>
       <c r="Z222" s="2"/>
     </row>
-    <row r="223">
+    <row r="223" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A223" s="3"/>
       <c r="B223" s="4"/>
       <c r="C223" s="5"/>
@@ -6862,7 +6911,7 @@
       <c r="Y223" s="2"/>
       <c r="Z223" s="2"/>
     </row>
-    <row r="224">
+    <row r="224" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A224" s="3"/>
       <c r="B224" s="4"/>
       <c r="C224" s="5"/>
@@ -6888,7 +6937,7 @@
       <c r="Y224" s="2"/>
       <c r="Z224" s="2"/>
     </row>
-    <row r="225">
+    <row r="225" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A225" s="3"/>
       <c r="B225" s="4"/>
       <c r="C225" s="5"/>
@@ -6914,7 +6963,7 @@
       <c r="Y225" s="2"/>
       <c r="Z225" s="2"/>
     </row>
-    <row r="226">
+    <row r="226" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A226" s="3"/>
       <c r="B226" s="4"/>
       <c r="C226" s="5"/>
@@ -6940,7 +6989,7 @@
       <c r="Y226" s="2"/>
       <c r="Z226" s="2"/>
     </row>
-    <row r="227">
+    <row r="227" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A227" s="3"/>
       <c r="B227" s="4"/>
       <c r="C227" s="5"/>
@@ -6966,7 +7015,7 @@
       <c r="Y227" s="2"/>
       <c r="Z227" s="2"/>
     </row>
-    <row r="228">
+    <row r="228" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A228" s="3"/>
       <c r="B228" s="4"/>
       <c r="C228" s="5"/>
@@ -6992,7 +7041,7 @@
       <c r="Y228" s="2"/>
       <c r="Z228" s="2"/>
     </row>
-    <row r="229">
+    <row r="229" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A229" s="3"/>
       <c r="B229" s="4"/>
       <c r="C229" s="5"/>
@@ -7018,7 +7067,7 @@
       <c r="Y229" s="2"/>
       <c r="Z229" s="2"/>
     </row>
-    <row r="230">
+    <row r="230" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A230" s="3"/>
       <c r="B230" s="4"/>
       <c r="C230" s="5"/>
@@ -7044,7 +7093,7 @@
       <c r="Y230" s="2"/>
       <c r="Z230" s="2"/>
     </row>
-    <row r="231">
+    <row r="231" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A231" s="3"/>
       <c r="B231" s="4"/>
       <c r="C231" s="5"/>
@@ -7070,7 +7119,7 @@
       <c r="Y231" s="2"/>
       <c r="Z231" s="2"/>
     </row>
-    <row r="232">
+    <row r="232" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A232" s="3"/>
       <c r="B232" s="4"/>
       <c r="C232" s="5"/>
@@ -7096,1372 +7145,1372 @@
       <c r="Y232" s="2"/>
       <c r="Z232" s="2"/>
     </row>
-    <row r="233">
+    <row r="233" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B233" s="8"/>
       <c r="C233" s="8"/>
       <c r="D233" s="8"/>
     </row>
-    <row r="234">
+    <row r="234" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B234" s="8"/>
       <c r="C234" s="8"/>
       <c r="D234" s="8"/>
     </row>
-    <row r="235">
+    <row r="235" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B235" s="8"/>
       <c r="C235" s="8"/>
       <c r="D235" s="8"/>
     </row>
-    <row r="236">
+    <row r="236" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B236" s="8"/>
       <c r="C236" s="8"/>
       <c r="D236" s="8"/>
     </row>
-    <row r="237">
+    <row r="237" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B237" s="8"/>
       <c r="C237" s="8"/>
       <c r="D237" s="8"/>
     </row>
-    <row r="238">
+    <row r="238" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B238" s="8"/>
       <c r="C238" s="8"/>
       <c r="D238" s="8"/>
     </row>
-    <row r="239">
+    <row r="239" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B239" s="8"/>
       <c r="C239" s="8"/>
       <c r="D239" s="8"/>
     </row>
-    <row r="240">
+    <row r="240" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B240" s="8"/>
       <c r="C240" s="8"/>
       <c r="D240" s="8"/>
     </row>
-    <row r="241">
+    <row r="241" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B241" s="8"/>
       <c r="C241" s="8"/>
       <c r="D241" s="8"/>
     </row>
-    <row r="242">
+    <row r="242" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B242" s="8"/>
       <c r="C242" s="8"/>
       <c r="D242" s="8"/>
     </row>
-    <row r="243">
+    <row r="243" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B243" s="8"/>
       <c r="C243" s="8"/>
       <c r="D243" s="8"/>
     </row>
-    <row r="244">
+    <row r="244" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B244" s="8"/>
       <c r="C244" s="8"/>
       <c r="D244" s="8"/>
     </row>
-    <row r="245">
+    <row r="245" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B245" s="8"/>
       <c r="C245" s="8"/>
       <c r="D245" s="8"/>
     </row>
-    <row r="246">
+    <row r="246" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B246" s="8"/>
       <c r="C246" s="8"/>
       <c r="D246" s="8"/>
     </row>
-    <row r="247">
+    <row r="247" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B247" s="8"/>
       <c r="C247" s="8"/>
       <c r="D247" s="8"/>
     </row>
-    <row r="248">
+    <row r="248" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B248" s="8"/>
       <c r="C248" s="8"/>
       <c r="D248" s="8"/>
     </row>
-    <row r="249">
+    <row r="249" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B249" s="8"/>
       <c r="C249" s="8"/>
       <c r="D249" s="8"/>
     </row>
-    <row r="250">
+    <row r="250" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B250" s="8"/>
       <c r="C250" s="8"/>
       <c r="D250" s="8"/>
     </row>
-    <row r="251">
+    <row r="251" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B251" s="8"/>
       <c r="C251" s="8"/>
       <c r="D251" s="8"/>
     </row>
-    <row r="252">
+    <row r="252" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B252" s="8"/>
       <c r="C252" s="8"/>
       <c r="D252" s="8"/>
     </row>
-    <row r="253">
+    <row r="253" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B253" s="8"/>
       <c r="C253" s="8"/>
       <c r="D253" s="8"/>
     </row>
-    <row r="254">
+    <row r="254" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B254" s="8"/>
       <c r="C254" s="8"/>
       <c r="D254" s="8"/>
     </row>
-    <row r="255">
+    <row r="255" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B255" s="8"/>
       <c r="C255" s="8"/>
       <c r="D255" s="8"/>
     </row>
-    <row r="256">
+    <row r="256" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B256" s="8"/>
       <c r="C256" s="8"/>
       <c r="D256" s="8"/>
     </row>
-    <row r="257">
+    <row r="257" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B257" s="8"/>
       <c r="C257" s="8"/>
       <c r="D257" s="8"/>
     </row>
-    <row r="258">
+    <row r="258" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B258" s="8"/>
       <c r="C258" s="8"/>
       <c r="D258" s="8"/>
     </row>
-    <row r="259">
+    <row r="259" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B259" s="8"/>
       <c r="C259" s="8"/>
       <c r="D259" s="8"/>
     </row>
-    <row r="260">
+    <row r="260" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B260" s="8"/>
       <c r="C260" s="8"/>
       <c r="D260" s="8"/>
     </row>
-    <row r="261">
+    <row r="261" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B261" s="8"/>
       <c r="C261" s="8"/>
       <c r="D261" s="8"/>
     </row>
-    <row r="262">
+    <row r="262" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B262" s="8"/>
       <c r="C262" s="8"/>
       <c r="D262" s="8"/>
     </row>
-    <row r="263">
+    <row r="263" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B263" s="8"/>
       <c r="C263" s="8"/>
       <c r="D263" s="8"/>
     </row>
-    <row r="264">
+    <row r="264" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B264" s="8"/>
       <c r="C264" s="8"/>
       <c r="D264" s="8"/>
     </row>
-    <row r="265">
+    <row r="265" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B265" s="8"/>
       <c r="C265" s="8"/>
       <c r="D265" s="8"/>
     </row>
-    <row r="266">
+    <row r="266" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B266" s="8"/>
       <c r="C266" s="8"/>
       <c r="D266" s="8"/>
     </row>
-    <row r="267">
+    <row r="267" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B267" s="8"/>
       <c r="C267" s="8"/>
       <c r="D267" s="8"/>
     </row>
-    <row r="268">
+    <row r="268" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B268" s="8"/>
       <c r="C268" s="8"/>
       <c r="D268" s="8"/>
     </row>
-    <row r="269">
+    <row r="269" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B269" s="8"/>
       <c r="C269" s="8"/>
       <c r="D269" s="8"/>
     </row>
-    <row r="270">
+    <row r="270" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B270" s="8"/>
       <c r="C270" s="8"/>
       <c r="D270" s="8"/>
     </row>
-    <row r="271">
+    <row r="271" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B271" s="8"/>
       <c r="C271" s="8"/>
       <c r="D271" s="8"/>
     </row>
-    <row r="272">
+    <row r="272" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B272" s="8"/>
       <c r="C272" s="8"/>
       <c r="D272" s="8"/>
     </row>
-    <row r="273">
+    <row r="273" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B273" s="8"/>
       <c r="C273" s="8"/>
       <c r="D273" s="8"/>
     </row>
-    <row r="274">
+    <row r="274" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B274" s="8"/>
       <c r="C274" s="8"/>
       <c r="D274" s="8"/>
     </row>
-    <row r="275">
+    <row r="275" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B275" s="8"/>
       <c r="C275" s="8"/>
       <c r="D275" s="8"/>
     </row>
-    <row r="276">
+    <row r="276" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B276" s="8"/>
       <c r="C276" s="8"/>
       <c r="D276" s="8"/>
     </row>
-    <row r="277">
+    <row r="277" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B277" s="8"/>
       <c r="C277" s="8"/>
       <c r="D277" s="8"/>
     </row>
-    <row r="278">
+    <row r="278" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B278" s="8"/>
       <c r="C278" s="8"/>
       <c r="D278" s="8"/>
     </row>
-    <row r="279">
+    <row r="279" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B279" s="8"/>
       <c r="C279" s="8"/>
       <c r="D279" s="8"/>
     </row>
-    <row r="280">
+    <row r="280" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B280" s="8"/>
       <c r="C280" s="8"/>
       <c r="D280" s="8"/>
     </row>
-    <row r="281">
+    <row r="281" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B281" s="8"/>
       <c r="C281" s="8"/>
       <c r="D281" s="8"/>
     </row>
-    <row r="282">
+    <row r="282" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B282" s="8"/>
       <c r="C282" s="8"/>
       <c r="D282" s="8"/>
     </row>
-    <row r="283">
+    <row r="283" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B283" s="8"/>
       <c r="C283" s="8"/>
       <c r="D283" s="8"/>
     </row>
-    <row r="284">
+    <row r="284" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B284" s="8"/>
       <c r="C284" s="8"/>
       <c r="D284" s="8"/>
     </row>
-    <row r="285">
+    <row r="285" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B285" s="8"/>
       <c r="C285" s="8"/>
       <c r="D285" s="8"/>
     </row>
-    <row r="286">
+    <row r="286" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B286" s="8"/>
       <c r="C286" s="8"/>
       <c r="D286" s="8"/>
     </row>
-    <row r="287">
+    <row r="287" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B287" s="8"/>
       <c r="C287" s="8"/>
       <c r="D287" s="8"/>
     </row>
-    <row r="288">
+    <row r="288" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B288" s="8"/>
       <c r="C288" s="8"/>
       <c r="D288" s="8"/>
     </row>
-    <row r="289">
+    <row r="289" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B289" s="8"/>
       <c r="C289" s="8"/>
       <c r="D289" s="8"/>
     </row>
-    <row r="290">
+    <row r="290" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B290" s="8"/>
       <c r="C290" s="8"/>
       <c r="D290" s="8"/>
     </row>
-    <row r="291">
+    <row r="291" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B291" s="8"/>
       <c r="C291" s="8"/>
       <c r="D291" s="8"/>
     </row>
-    <row r="292">
+    <row r="292" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B292" s="8"/>
       <c r="C292" s="8"/>
       <c r="D292" s="8"/>
     </row>
-    <row r="293">
+    <row r="293" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B293" s="8"/>
       <c r="C293" s="8"/>
       <c r="D293" s="8"/>
     </row>
-    <row r="294">
+    <row r="294" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B294" s="8"/>
       <c r="C294" s="8"/>
       <c r="D294" s="8"/>
     </row>
-    <row r="295">
+    <row r="295" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B295" s="8"/>
       <c r="C295" s="8"/>
       <c r="D295" s="8"/>
     </row>
-    <row r="296">
+    <row r="296" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B296" s="8"/>
       <c r="C296" s="8"/>
       <c r="D296" s="8"/>
     </row>
-    <row r="297">
+    <row r="297" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B297" s="8"/>
       <c r="C297" s="8"/>
       <c r="D297" s="8"/>
     </row>
-    <row r="298">
+    <row r="298" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B298" s="8"/>
       <c r="C298" s="8"/>
       <c r="D298" s="8"/>
     </row>
-    <row r="299">
+    <row r="299" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B299" s="8"/>
       <c r="C299" s="8"/>
       <c r="D299" s="8"/>
     </row>
-    <row r="300">
+    <row r="300" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B300" s="8"/>
       <c r="C300" s="8"/>
       <c r="D300" s="8"/>
     </row>
-    <row r="301">
+    <row r="301" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B301" s="8"/>
       <c r="C301" s="8"/>
       <c r="D301" s="8"/>
     </row>
-    <row r="302">
+    <row r="302" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B302" s="8"/>
       <c r="C302" s="8"/>
       <c r="D302" s="8"/>
     </row>
-    <row r="303">
+    <row r="303" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B303" s="8"/>
       <c r="C303" s="8"/>
       <c r="D303" s="8"/>
     </row>
-    <row r="304">
+    <row r="304" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B304" s="8"/>
       <c r="C304" s="8"/>
       <c r="D304" s="8"/>
     </row>
-    <row r="305">
+    <row r="305" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B305" s="8"/>
       <c r="C305" s="8"/>
       <c r="D305" s="8"/>
     </row>
-    <row r="306">
+    <row r="306" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B306" s="8"/>
       <c r="C306" s="8"/>
       <c r="D306" s="8"/>
     </row>
-    <row r="307">
+    <row r="307" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B307" s="8"/>
       <c r="C307" s="8"/>
       <c r="D307" s="8"/>
     </row>
-    <row r="308">
+    <row r="308" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B308" s="8"/>
       <c r="C308" s="8"/>
       <c r="D308" s="8"/>
     </row>
-    <row r="309">
+    <row r="309" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B309" s="8"/>
       <c r="C309" s="8"/>
       <c r="D309" s="8"/>
     </row>
-    <row r="310">
+    <row r="310" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B310" s="8"/>
       <c r="C310" s="8"/>
       <c r="D310" s="8"/>
     </row>
-    <row r="311">
+    <row r="311" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B311" s="8"/>
       <c r="C311" s="8"/>
       <c r="D311" s="8"/>
     </row>
-    <row r="312">
+    <row r="312" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B312" s="8"/>
       <c r="C312" s="8"/>
       <c r="D312" s="8"/>
     </row>
-    <row r="313">
+    <row r="313" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B313" s="8"/>
       <c r="C313" s="8"/>
       <c r="D313" s="8"/>
     </row>
-    <row r="314">
+    <row r="314" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B314" s="8"/>
       <c r="C314" s="8"/>
       <c r="D314" s="8"/>
     </row>
-    <row r="315">
+    <row r="315" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B315" s="8"/>
       <c r="C315" s="8"/>
       <c r="D315" s="8"/>
     </row>
-    <row r="316">
+    <row r="316" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B316" s="8"/>
       <c r="C316" s="8"/>
       <c r="D316" s="8"/>
     </row>
-    <row r="317">
+    <row r="317" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B317" s="8"/>
       <c r="C317" s="8"/>
       <c r="D317" s="8"/>
     </row>
-    <row r="318">
+    <row r="318" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B318" s="8"/>
       <c r="C318" s="8"/>
       <c r="D318" s="8"/>
     </row>
-    <row r="319">
+    <row r="319" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B319" s="8"/>
       <c r="C319" s="8"/>
       <c r="D319" s="8"/>
     </row>
-    <row r="320">
+    <row r="320" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B320" s="8"/>
       <c r="C320" s="8"/>
       <c r="D320" s="8"/>
     </row>
-    <row r="321">
+    <row r="321" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B321" s="8"/>
       <c r="C321" s="8"/>
       <c r="D321" s="8"/>
     </row>
-    <row r="322">
+    <row r="322" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B322" s="8"/>
       <c r="C322" s="8"/>
       <c r="D322" s="8"/>
     </row>
-    <row r="323">
+    <row r="323" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B323" s="8"/>
       <c r="C323" s="8"/>
       <c r="D323" s="8"/>
     </row>
-    <row r="324">
+    <row r="324" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B324" s="8"/>
       <c r="C324" s="8"/>
       <c r="D324" s="8"/>
     </row>
-    <row r="325">
+    <row r="325" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B325" s="8"/>
       <c r="C325" s="8"/>
       <c r="D325" s="8"/>
     </row>
-    <row r="326">
+    <row r="326" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B326" s="8"/>
       <c r="C326" s="8"/>
       <c r="D326" s="8"/>
     </row>
-    <row r="327">
+    <row r="327" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B327" s="8"/>
       <c r="C327" s="8"/>
       <c r="D327" s="8"/>
     </row>
-    <row r="328">
+    <row r="328" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B328" s="8"/>
       <c r="C328" s="8"/>
       <c r="D328" s="8"/>
     </row>
-    <row r="329">
+    <row r="329" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B329" s="8"/>
       <c r="C329" s="8"/>
       <c r="D329" s="8"/>
     </row>
-    <row r="330">
+    <row r="330" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B330" s="8"/>
       <c r="C330" s="8"/>
       <c r="D330" s="8"/>
     </row>
-    <row r="331">
+    <row r="331" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B331" s="8"/>
       <c r="C331" s="8"/>
       <c r="D331" s="8"/>
     </row>
-    <row r="332">
+    <row r="332" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B332" s="8"/>
       <c r="C332" s="8"/>
       <c r="D332" s="8"/>
     </row>
-    <row r="333">
+    <row r="333" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B333" s="8"/>
       <c r="C333" s="8"/>
       <c r="D333" s="8"/>
     </row>
-    <row r="334">
+    <row r="334" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B334" s="8"/>
       <c r="C334" s="8"/>
       <c r="D334" s="8"/>
     </row>
-    <row r="335">
+    <row r="335" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B335" s="8"/>
       <c r="C335" s="8"/>
       <c r="D335" s="8"/>
     </row>
-    <row r="336">
+    <row r="336" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B336" s="8"/>
       <c r="C336" s="8"/>
       <c r="D336" s="8"/>
     </row>
-    <row r="337">
+    <row r="337" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B337" s="8"/>
       <c r="C337" s="8"/>
       <c r="D337" s="8"/>
     </row>
-    <row r="338">
+    <row r="338" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B338" s="8"/>
       <c r="C338" s="8"/>
       <c r="D338" s="8"/>
     </row>
-    <row r="339">
+    <row r="339" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B339" s="8"/>
       <c r="C339" s="8"/>
       <c r="D339" s="8"/>
     </row>
-    <row r="340">
+    <row r="340" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B340" s="8"/>
       <c r="C340" s="8"/>
       <c r="D340" s="8"/>
     </row>
-    <row r="341">
+    <row r="341" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B341" s="8"/>
       <c r="C341" s="8"/>
       <c r="D341" s="8"/>
     </row>
-    <row r="342">
+    <row r="342" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B342" s="8"/>
       <c r="C342" s="8"/>
       <c r="D342" s="8"/>
     </row>
-    <row r="343">
+    <row r="343" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B343" s="8"/>
       <c r="C343" s="8"/>
       <c r="D343" s="8"/>
     </row>
-    <row r="344">
+    <row r="344" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B344" s="8"/>
       <c r="C344" s="8"/>
       <c r="D344" s="8"/>
     </row>
-    <row r="345">
+    <row r="345" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B345" s="8"/>
       <c r="C345" s="8"/>
       <c r="D345" s="8"/>
     </row>
-    <row r="346">
+    <row r="346" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B346" s="8"/>
       <c r="C346" s="8"/>
       <c r="D346" s="8"/>
     </row>
-    <row r="347">
+    <row r="347" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B347" s="8"/>
       <c r="C347" s="8"/>
       <c r="D347" s="8"/>
     </row>
-    <row r="348">
+    <row r="348" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B348" s="8"/>
       <c r="C348" s="8"/>
       <c r="D348" s="8"/>
     </row>
-    <row r="349">
+    <row r="349" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B349" s="8"/>
       <c r="C349" s="8"/>
       <c r="D349" s="8"/>
     </row>
-    <row r="350">
+    <row r="350" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B350" s="8"/>
       <c r="C350" s="8"/>
       <c r="D350" s="8"/>
     </row>
-    <row r="351">
+    <row r="351" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B351" s="8"/>
       <c r="C351" s="8"/>
       <c r="D351" s="8"/>
     </row>
-    <row r="352">
+    <row r="352" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B352" s="8"/>
       <c r="C352" s="8"/>
       <c r="D352" s="8"/>
     </row>
-    <row r="353">
+    <row r="353" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B353" s="8"/>
       <c r="C353" s="8"/>
       <c r="D353" s="8"/>
     </row>
-    <row r="354">
+    <row r="354" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B354" s="8"/>
       <c r="C354" s="8"/>
       <c r="D354" s="8"/>
     </row>
-    <row r="355">
+    <row r="355" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B355" s="8"/>
       <c r="C355" s="8"/>
       <c r="D355" s="8"/>
     </row>
-    <row r="356">
+    <row r="356" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B356" s="8"/>
       <c r="C356" s="8"/>
       <c r="D356" s="8"/>
     </row>
-    <row r="357">
+    <row r="357" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B357" s="8"/>
       <c r="C357" s="8"/>
       <c r="D357" s="8"/>
     </row>
-    <row r="358">
+    <row r="358" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B358" s="8"/>
       <c r="C358" s="8"/>
       <c r="D358" s="8"/>
     </row>
-    <row r="359">
+    <row r="359" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B359" s="8"/>
       <c r="C359" s="8"/>
       <c r="D359" s="8"/>
     </row>
-    <row r="360">
+    <row r="360" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B360" s="8"/>
       <c r="C360" s="8"/>
       <c r="D360" s="8"/>
     </row>
-    <row r="361">
+    <row r="361" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B361" s="8"/>
       <c r="C361" s="8"/>
       <c r="D361" s="8"/>
     </row>
-    <row r="362">
+    <row r="362" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B362" s="8"/>
       <c r="C362" s="8"/>
       <c r="D362" s="8"/>
     </row>
-    <row r="363">
+    <row r="363" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B363" s="8"/>
       <c r="C363" s="8"/>
       <c r="D363" s="8"/>
     </row>
-    <row r="364">
+    <row r="364" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B364" s="8"/>
       <c r="C364" s="8"/>
       <c r="D364" s="8"/>
     </row>
-    <row r="365">
+    <row r="365" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B365" s="8"/>
       <c r="C365" s="8"/>
       <c r="D365" s="8"/>
     </row>
-    <row r="366">
+    <row r="366" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B366" s="8"/>
       <c r="C366" s="8"/>
       <c r="D366" s="8"/>
     </row>
-    <row r="367">
+    <row r="367" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B367" s="8"/>
       <c r="C367" s="8"/>
       <c r="D367" s="8"/>
     </row>
-    <row r="368">
+    <row r="368" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B368" s="8"/>
       <c r="C368" s="8"/>
       <c r="D368" s="8"/>
     </row>
-    <row r="369">
+    <row r="369" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B369" s="8"/>
       <c r="C369" s="8"/>
       <c r="D369" s="8"/>
     </row>
-    <row r="370">
+    <row r="370" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B370" s="8"/>
       <c r="C370" s="8"/>
       <c r="D370" s="8"/>
     </row>
-    <row r="371">
+    <row r="371" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B371" s="8"/>
       <c r="C371" s="8"/>
       <c r="D371" s="8"/>
     </row>
-    <row r="372">
+    <row r="372" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B372" s="8"/>
       <c r="C372" s="8"/>
       <c r="D372" s="8"/>
     </row>
-    <row r="373">
+    <row r="373" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B373" s="8"/>
       <c r="C373" s="8"/>
       <c r="D373" s="8"/>
     </row>
-    <row r="374">
+    <row r="374" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B374" s="8"/>
       <c r="C374" s="8"/>
       <c r="D374" s="8"/>
     </row>
-    <row r="375">
+    <row r="375" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B375" s="8"/>
       <c r="C375" s="8"/>
       <c r="D375" s="8"/>
     </row>
-    <row r="376">
+    <row r="376" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B376" s="8"/>
       <c r="C376" s="8"/>
       <c r="D376" s="8"/>
     </row>
-    <row r="377">
+    <row r="377" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B377" s="8"/>
       <c r="C377" s="8"/>
       <c r="D377" s="8"/>
     </row>
-    <row r="378">
+    <row r="378" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B378" s="8"/>
       <c r="C378" s="8"/>
       <c r="D378" s="8"/>
     </row>
-    <row r="379">
+    <row r="379" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B379" s="8"/>
       <c r="C379" s="8"/>
       <c r="D379" s="8"/>
     </row>
-    <row r="380">
+    <row r="380" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B380" s="8"/>
       <c r="C380" s="8"/>
       <c r="D380" s="8"/>
     </row>
-    <row r="381">
+    <row r="381" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B381" s="8"/>
       <c r="C381" s="8"/>
       <c r="D381" s="8"/>
     </row>
-    <row r="382">
+    <row r="382" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B382" s="8"/>
       <c r="C382" s="8"/>
       <c r="D382" s="8"/>
     </row>
-    <row r="383">
+    <row r="383" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B383" s="8"/>
       <c r="C383" s="8"/>
       <c r="D383" s="8"/>
     </row>
-    <row r="384">
+    <row r="384" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B384" s="8"/>
       <c r="C384" s="8"/>
       <c r="D384" s="8"/>
     </row>
-    <row r="385">
+    <row r="385" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B385" s="8"/>
       <c r="C385" s="8"/>
       <c r="D385" s="8"/>
     </row>
-    <row r="386">
+    <row r="386" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B386" s="8"/>
       <c r="C386" s="8"/>
       <c r="D386" s="8"/>
     </row>
-    <row r="387">
+    <row r="387" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B387" s="8"/>
       <c r="C387" s="8"/>
       <c r="D387" s="8"/>
     </row>
-    <row r="388">
+    <row r="388" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B388" s="8"/>
       <c r="C388" s="8"/>
       <c r="D388" s="8"/>
     </row>
-    <row r="389">
+    <row r="389" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B389" s="8"/>
       <c r="C389" s="8"/>
       <c r="D389" s="8"/>
     </row>
-    <row r="390">
+    <row r="390" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B390" s="8"/>
       <c r="C390" s="8"/>
       <c r="D390" s="8"/>
     </row>
-    <row r="391">
+    <row r="391" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B391" s="8"/>
       <c r="C391" s="8"/>
       <c r="D391" s="8"/>
     </row>
-    <row r="392">
+    <row r="392" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B392" s="8"/>
       <c r="C392" s="8"/>
       <c r="D392" s="8"/>
     </row>
-    <row r="393">
+    <row r="393" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B393" s="8"/>
       <c r="C393" s="8"/>
       <c r="D393" s="8"/>
     </row>
-    <row r="394">
+    <row r="394" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B394" s="8"/>
       <c r="C394" s="8"/>
       <c r="D394" s="8"/>
     </row>
-    <row r="395">
+    <row r="395" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B395" s="8"/>
       <c r="C395" s="8"/>
       <c r="D395" s="8"/>
     </row>
-    <row r="396">
+    <row r="396" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B396" s="8"/>
       <c r="C396" s="8"/>
       <c r="D396" s="8"/>
     </row>
-    <row r="397">
+    <row r="397" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B397" s="8"/>
       <c r="C397" s="8"/>
       <c r="D397" s="8"/>
     </row>
-    <row r="398">
+    <row r="398" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B398" s="8"/>
       <c r="C398" s="8"/>
       <c r="D398" s="8"/>
     </row>
-    <row r="399">
+    <row r="399" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B399" s="8"/>
       <c r="C399" s="8"/>
       <c r="D399" s="8"/>
     </row>
-    <row r="400">
+    <row r="400" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B400" s="8"/>
       <c r="C400" s="8"/>
       <c r="D400" s="8"/>
     </row>
-    <row r="401">
+    <row r="401" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B401" s="8"/>
       <c r="C401" s="8"/>
       <c r="D401" s="8"/>
     </row>
-    <row r="402">
+    <row r="402" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B402" s="8"/>
       <c r="C402" s="8"/>
       <c r="D402" s="8"/>
     </row>
-    <row r="403">
+    <row r="403" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B403" s="8"/>
       <c r="C403" s="8"/>
       <c r="D403" s="8"/>
     </row>
-    <row r="404">
+    <row r="404" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B404" s="8"/>
       <c r="C404" s="8"/>
       <c r="D404" s="8"/>
     </row>
-    <row r="405">
+    <row r="405" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B405" s="8"/>
       <c r="C405" s="8"/>
       <c r="D405" s="8"/>
     </row>
-    <row r="406">
+    <row r="406" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B406" s="8"/>
       <c r="C406" s="8"/>
       <c r="D406" s="8"/>
     </row>
-    <row r="407">
+    <row r="407" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B407" s="8"/>
       <c r="C407" s="8"/>
       <c r="D407" s="8"/>
     </row>
-    <row r="408">
+    <row r="408" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B408" s="8"/>
       <c r="C408" s="8"/>
       <c r="D408" s="8"/>
     </row>
-    <row r="409">
+    <row r="409" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B409" s="8"/>
       <c r="C409" s="8"/>
       <c r="D409" s="8"/>
     </row>
-    <row r="410">
+    <row r="410" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B410" s="8"/>
       <c r="C410" s="8"/>
       <c r="D410" s="8"/>
     </row>
-    <row r="411">
+    <row r="411" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B411" s="8"/>
       <c r="C411" s="8"/>
       <c r="D411" s="8"/>
     </row>
-    <row r="412">
+    <row r="412" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B412" s="8"/>
       <c r="C412" s="8"/>
       <c r="D412" s="8"/>
     </row>
-    <row r="413">
+    <row r="413" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B413" s="8"/>
       <c r="C413" s="8"/>
       <c r="D413" s="8"/>
     </row>
-    <row r="414">
+    <row r="414" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B414" s="8"/>
       <c r="C414" s="8"/>
       <c r="D414" s="8"/>
     </row>
-    <row r="415">
+    <row r="415" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B415" s="8"/>
       <c r="C415" s="8"/>
       <c r="D415" s="8"/>
     </row>
-    <row r="416">
+    <row r="416" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B416" s="8"/>
       <c r="C416" s="8"/>
       <c r="D416" s="8"/>
     </row>
-    <row r="417">
+    <row r="417" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B417" s="8"/>
       <c r="C417" s="8"/>
       <c r="D417" s="8"/>
     </row>
-    <row r="418">
+    <row r="418" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B418" s="8"/>
       <c r="C418" s="8"/>
       <c r="D418" s="8"/>
     </row>
-    <row r="419">
+    <row r="419" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B419" s="8"/>
       <c r="C419" s="8"/>
       <c r="D419" s="8"/>
     </row>
-    <row r="420">
+    <row r="420" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B420" s="8"/>
       <c r="C420" s="8"/>
       <c r="D420" s="8"/>
     </row>
-    <row r="421">
+    <row r="421" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B421" s="8"/>
       <c r="C421" s="8"/>
       <c r="D421" s="8"/>
     </row>
-    <row r="422">
+    <row r="422" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B422" s="8"/>
       <c r="C422" s="8"/>
       <c r="D422" s="8"/>
     </row>
-    <row r="423">
+    <row r="423" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B423" s="8"/>
       <c r="C423" s="8"/>
       <c r="D423" s="8"/>
     </row>
-    <row r="424">
+    <row r="424" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B424" s="8"/>
       <c r="C424" s="8"/>
       <c r="D424" s="8"/>
     </row>
-    <row r="425">
+    <row r="425" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B425" s="8"/>
       <c r="C425" s="8"/>
       <c r="D425" s="8"/>
     </row>
-    <row r="426">
+    <row r="426" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B426" s="8"/>
       <c r="C426" s="8"/>
       <c r="D426" s="8"/>
     </row>
-    <row r="427">
+    <row r="427" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B427" s="8"/>
       <c r="C427" s="8"/>
       <c r="D427" s="8"/>
     </row>
-    <row r="428">
+    <row r="428" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B428" s="8"/>
       <c r="C428" s="8"/>
       <c r="D428" s="8"/>
     </row>
-    <row r="429">
+    <row r="429" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B429" s="8"/>
       <c r="C429" s="8"/>
       <c r="D429" s="8"/>
     </row>
-    <row r="430">
+    <row r="430" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B430" s="8"/>
       <c r="C430" s="8"/>
     </row>
-    <row r="431">
+    <row r="431" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B431" s="8"/>
       <c r="C431" s="8"/>
     </row>
-    <row r="432">
+    <row r="432" spans="2:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B432" s="8"/>
       <c r="C432" s="8"/>
     </row>
-    <row r="433">
+    <row r="433" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B433" s="8"/>
       <c r="C433" s="8"/>
     </row>
-    <row r="434">
+    <row r="434" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B434" s="8"/>
       <c r="C434" s="8"/>
     </row>
-    <row r="435">
+    <row r="435" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B435" s="8"/>
       <c r="C435" s="8"/>
     </row>
-    <row r="436">
+    <row r="436" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B436" s="8"/>
       <c r="C436" s="8"/>
     </row>
-    <row r="437">
+    <row r="437" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B437" s="8"/>
       <c r="C437" s="8"/>
     </row>
-    <row r="438">
+    <row r="438" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B438" s="8"/>
       <c r="C438" s="8"/>
     </row>
-    <row r="439">
+    <row r="439" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B439" s="8"/>
       <c r="C439" s="8"/>
     </row>
-    <row r="440">
+    <row r="440" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B440" s="8"/>
       <c r="C440" s="8"/>
     </row>
-    <row r="441">
+    <row r="441" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B441" s="8"/>
       <c r="C441" s="8"/>
     </row>
-    <row r="442">
+    <row r="442" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B442" s="8"/>
       <c r="C442" s="8"/>
     </row>
-    <row r="443">
+    <row r="443" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B443" s="8"/>
       <c r="C443" s="8"/>
     </row>
-    <row r="444">
+    <row r="444" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B444" s="8"/>
       <c r="C444" s="8"/>
     </row>
-    <row r="445">
+    <row r="445" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B445" s="8"/>
       <c r="C445" s="8"/>
     </row>
-    <row r="446">
+    <row r="446" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B446" s="8"/>
       <c r="C446" s="8"/>
     </row>
-    <row r="447">
+    <row r="447" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B447" s="8"/>
       <c r="C447" s="8"/>
     </row>
-    <row r="448">
+    <row r="448" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B448" s="8"/>
       <c r="C448" s="8"/>
     </row>
-    <row r="449">
+    <row r="449" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B449" s="8"/>
       <c r="C449" s="8"/>
     </row>
-    <row r="450">
+    <row r="450" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B450" s="8"/>
       <c r="C450" s="8"/>
     </row>
-    <row r="451">
+    <row r="451" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B451" s="8"/>
       <c r="C451" s="8"/>
     </row>
-    <row r="452">
+    <row r="452" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B452" s="8"/>
       <c r="C452" s="8"/>
     </row>
-    <row r="453">
+    <row r="453" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B453" s="8"/>
       <c r="C453" s="8"/>
     </row>
-    <row r="454">
+    <row r="454" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B454" s="8"/>
       <c r="C454" s="8"/>
     </row>
-    <row r="455">
+    <row r="455" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B455" s="8"/>
       <c r="C455" s="8"/>
     </row>
-    <row r="456">
+    <row r="456" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B456" s="8"/>
       <c r="C456" s="8"/>
     </row>
-    <row r="457">
+    <row r="457" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B457" s="8"/>
       <c r="C457" s="8"/>
     </row>
-    <row r="458">
+    <row r="458" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B458" s="8"/>
       <c r="C458" s="8"/>
     </row>
-    <row r="459">
+    <row r="459" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B459" s="8"/>
       <c r="C459" s="8"/>
     </row>
-    <row r="460">
+    <row r="460" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B460" s="8"/>
       <c r="C460" s="8"/>
     </row>
-    <row r="461">
+    <row r="461" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B461" s="8"/>
       <c r="C461" s="8"/>
     </row>
-    <row r="462">
+    <row r="462" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B462" s="8"/>
       <c r="C462" s="8"/>
     </row>
-    <row r="463">
+    <row r="463" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B463" s="8"/>
       <c r="C463" s="8"/>
     </row>
-    <row r="464">
+    <row r="464" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B464" s="8"/>
       <c r="C464" s="8"/>
     </row>
-    <row r="465">
+    <row r="465" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B465" s="8"/>
       <c r="C465" s="8"/>
     </row>
-    <row r="466">
+    <row r="466" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B466" s="8"/>
       <c r="C466" s="8"/>
     </row>
-    <row r="467">
+    <row r="467" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B467" s="8"/>
       <c r="C467" s="8"/>
     </row>
-    <row r="468">
+    <row r="468" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B468" s="8"/>
       <c r="C468" s="8"/>
     </row>
-    <row r="469">
+    <row r="469" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B469" s="8"/>
       <c r="C469" s="8"/>
     </row>
-    <row r="470">
+    <row r="470" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B470" s="8"/>
       <c r="C470" s="8"/>
     </row>
-    <row r="471">
+    <row r="471" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B471" s="8"/>
       <c r="C471" s="8"/>
     </row>
-    <row r="472">
+    <row r="472" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B472" s="8"/>
       <c r="C472" s="8"/>
     </row>
-    <row r="473">
+    <row r="473" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B473" s="8"/>
       <c r="C473" s="8"/>
     </row>
-    <row r="474">
+    <row r="474" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B474" s="8"/>
       <c r="C474" s="8"/>
     </row>
-    <row r="475">
+    <row r="475" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B475" s="8"/>
       <c r="C475" s="8"/>
     </row>
-    <row r="476">
+    <row r="476" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B476" s="8"/>
       <c r="C476" s="8"/>
     </row>
-    <row r="477">
+    <row r="477" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B477" s="8"/>
       <c r="C477" s="8"/>
     </row>
-    <row r="478">
+    <row r="478" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B478" s="8"/>
       <c r="C478" s="8"/>
     </row>
-    <row r="479">
+    <row r="479" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B479" s="8"/>
       <c r="C479" s="8"/>
     </row>
-    <row r="480">
+    <row r="480" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B480" s="8"/>
       <c r="C480" s="8"/>
     </row>
-    <row r="481">
+    <row r="481" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B481" s="8"/>
       <c r="C481" s="8"/>
     </row>
-    <row r="482">
+    <row r="482" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B482" s="8"/>
       <c r="C482" s="8"/>
     </row>
-    <row r="483">
+    <row r="483" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B483" s="8"/>
       <c r="C483" s="8"/>
     </row>
-    <row r="484">
+    <row r="484" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B484" s="8"/>
       <c r="C484" s="8"/>
     </row>
-    <row r="485">
+    <row r="485" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B485" s="8"/>
       <c r="C485" s="8"/>
     </row>
-    <row r="486">
+    <row r="486" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B486" s="8"/>
       <c r="C486" s="8"/>
     </row>
-    <row r="487">
+    <row r="487" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B487" s="8"/>
       <c r="C487" s="8"/>
     </row>
-    <row r="488">
+    <row r="488" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B488" s="8"/>
       <c r="C488" s="8"/>
     </row>
-    <row r="489">
+    <row r="489" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B489" s="8"/>
       <c r="C489" s="8"/>
     </row>
-    <row r="490">
+    <row r="490" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B490" s="8"/>
       <c r="C490" s="8"/>
     </row>
-    <row r="491">
+    <row r="491" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B491" s="8"/>
       <c r="C491" s="8"/>
     </row>
-    <row r="492">
+    <row r="492" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B492" s="8"/>
       <c r="C492" s="8"/>
     </row>
-    <row r="493">
+    <row r="493" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B493" s="8"/>
       <c r="C493" s="8"/>
     </row>
-    <row r="494">
+    <row r="494" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B494" s="8"/>
       <c r="C494" s="8"/>
     </row>
-    <row r="495">
+    <row r="495" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B495" s="8"/>
       <c r="C495" s="8"/>
     </row>
-    <row r="496">
+    <row r="496" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B496" s="8"/>
       <c r="C496" s="8"/>
     </row>
-    <row r="497">
+    <row r="497" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B497" s="8"/>
       <c r="C497" s="8"/>
     </row>
-    <row r="498">
+    <row r="498" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B498" s="8"/>
       <c r="C498" s="8"/>
     </row>
-    <row r="499">
+    <row r="499" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B499" s="8"/>
       <c r="C499" s="8"/>
     </row>
-    <row r="500">
+    <row r="500" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B500" s="8"/>
       <c r="C500" s="8"/>
     </row>
-    <row r="501">
+    <row r="501" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B501" s="8"/>
       <c r="C501" s="8"/>
     </row>
-    <row r="502">
+    <row r="502" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B502" s="8"/>
       <c r="C502" s="8"/>
     </row>
-    <row r="503">
+    <row r="503" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B503" s="8"/>
       <c r="C503" s="8"/>
     </row>
-    <row r="504">
+    <row r="504" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B504" s="8"/>
       <c r="C504" s="8"/>
     </row>
-    <row r="505">
+    <row r="505" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B505" s="8"/>
       <c r="C505" s="8"/>
     </row>
-    <row r="506">
+    <row r="506" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B506" s="8"/>
       <c r="C506" s="8"/>
     </row>
-    <row r="507">
+    <row r="507" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B507" s="8"/>
       <c r="C507" s="8"/>
     </row>
-    <row r="508">
+    <row r="508" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B508" s="8"/>
       <c r="C508" s="8"/>
     </row>
-    <row r="509">
+    <row r="509" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B509" s="8"/>
       <c r="C509" s="8"/>
     </row>
-    <row r="510">
+    <row r="510" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B510" s="8"/>
       <c r="C510" s="8"/>
     </row>
-    <row r="511">
+    <row r="511" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B511" s="8"/>
       <c r="C511" s="8"/>
     </row>
-    <row r="512">
+    <row r="512" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B512" s="8"/>
       <c r="C512" s="8"/>
     </row>
-    <row r="513">
+    <row r="513" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B513" s="8"/>
       <c r="C513" s="8"/>
     </row>
-    <row r="514">
+    <row r="514" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B514" s="8"/>
       <c r="C514" s="8"/>
     </row>
-    <row r="515">
+    <row r="515" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B515" s="8"/>
       <c r="C515" s="8"/>
     </row>
-    <row r="516">
+    <row r="516" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B516" s="8"/>
       <c r="C516" s="8"/>
     </row>
-    <row r="517">
+    <row r="517" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B517" s="8"/>
       <c r="C517" s="8"/>
     </row>
-    <row r="518">
+    <row r="518" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B518" s="8"/>
       <c r="C518" s="8"/>
     </row>
-    <row r="519">
+    <row r="519" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B519" s="8"/>
       <c r="C519" s="8"/>
     </row>
-    <row r="520">
+    <row r="520" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B520" s="8"/>
       <c r="C520" s="8"/>
     </row>
-    <row r="521">
+    <row r="521" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B521" s="8"/>
       <c r="C521" s="8"/>
     </row>
-    <row r="522">
+    <row r="522" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B522" s="8"/>
       <c r="C522" s="8"/>
     </row>
-    <row r="523">
+    <row r="523" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B523" s="8"/>
       <c r="C523" s="8"/>
     </row>
-    <row r="524">
+    <row r="524" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B524" s="8"/>
       <c r="C524" s="8"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>